<commit_message>
[#8049] add a new absent reason (disaster)
</commit_message>
<xml_diff>
--- a/storage/app/excel/child_application_table.xlsx
+++ b/storage/app/excel/child_application_table.xlsx
@@ -14,21 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
+  <si>
+    <t>合計</t>
+  </si>
   <si>
     <t>定員</t>
   </si>
   <si>
     <t>19名</t>
-  </si>
-  <si>
-    <t>合計</t>
-  </si>
-  <si>
-    <t>0歳児</t>
-  </si>
-  <si>
-    <t>従業員枠</t>
   </si>
   <si>
     <t>延長時間</t>
@@ -40,16 +34,28 @@
     <t>A</t>
   </si>
   <si>
+    <t>0歳児</t>
+  </si>
+  <si>
+    <t>従業員枠</t>
+  </si>
+  <si>
+    <t>18:31～19:00</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
     <t>1歳児</t>
   </si>
   <si>
     <t>地域枠</t>
   </si>
   <si>
-    <t>18:31～19:00</t>
+    <t>19:01～19:30</t>
   </si>
   <si>
-    <t>B</t>
+    <t>C</t>
   </si>
   <si>
     <t>2歳児</t>
@@ -59,19 +65,19 @@
 割合</t>
   </si>
   <si>
-    <t>19:01～19:30</t>
+    <t>19:31～20:00</t>
   </si>
   <si>
-    <t>C</t>
+    <t>D</t>
   </si>
   <si>
     <t>3歳児</t>
   </si>
   <si>
-    <t>19:31～20:00</t>
+    <t>それ以外</t>
   </si>
   <si>
-    <t>D</t>
+    <t>E</t>
   </si>
   <si>
     <t>4歳児</t>
@@ -81,15 +87,6 @@
 割合</t>
   </si>
   <si>
-    <t>それ以外</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>5歳児</t>
-  </si>
-  <si>
     <t>欠席など</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>コ</t>
+  </si>
+  <si>
+    <t>5歳児</t>
   </si>
   <si>
     <t>都合欠席</t>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>休</t>
+  </si>
+  <si>
+    <t>災害</t>
+  </si>
+  <si>
+    <t>災</t>
   </si>
   <si>
     <t>登園
@@ -212,9 +218,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -271,22 +277,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -302,9 +292,93 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,75 +393,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,7 +401,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -447,7 +453,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,7 +471,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,7 +489,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,13 +519,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,7 +537,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,43 +579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,13 +591,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,36 +609,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -691,12 +697,61 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -783,6 +838,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -794,6 +858,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -815,33 +912,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -850,27 +920,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -888,134 +943,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1107,8 +1162,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1119,18 +1189,24 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1140,22 +1216,28 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1167,26 +1249,44 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1507,10 +1607,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:CI203"/>
+  <dimension ref="A1:CJ203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="CB30" sqref="CB30"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AH10" sqref="AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1540,9 +1640,42 @@
       <c r="CH1" s="3"/>
       <c r="CI1" s="3"/>
     </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="75:87">
-      <c r="BW2" s="3"/>
-      <c r="BX2" s="3"/>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="44:87">
+      <c r="AR2" s="37"/>
+      <c r="AS2" s="37"/>
+      <c r="AT2" s="37"/>
+      <c r="AU2" s="37"/>
+      <c r="AV2" s="37"/>
+      <c r="AW2" s="37"/>
+      <c r="AX2" s="37"/>
+      <c r="AY2" s="37"/>
+      <c r="AZ2" s="37"/>
+      <c r="BA2" s="37"/>
+      <c r="BB2" s="37"/>
+      <c r="BC2" s="37"/>
+      <c r="BD2" s="37"/>
+      <c r="BE2" s="37"/>
+      <c r="BF2" s="37"/>
+      <c r="BG2" s="37"/>
+      <c r="BH2" s="37"/>
+      <c r="BI2" s="37"/>
+      <c r="BJ2" s="37"/>
+      <c r="BK2" s="37"/>
+      <c r="BL2" s="37"/>
+      <c r="BM2" s="37"/>
+      <c r="BN2" s="37"/>
+      <c r="BO2" s="37"/>
+      <c r="BP2" s="37"/>
+      <c r="BQ2" s="37"/>
+      <c r="BR2" s="37"/>
+      <c r="BS2" s="37"/>
+      <c r="BT2" s="37"/>
+      <c r="BU2" s="37"/>
+      <c r="BV2" s="51"/>
+      <c r="BW2" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX2" s="37"/>
       <c r="BY2" s="3"/>
       <c r="BZ2" s="3"/>
       <c r="CA2" s="3"/>
@@ -1570,49 +1703,47 @@
       <c r="K3" s="7"/>
       <c r="L3" s="21"/>
       <c r="M3" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="9"/>
       <c r="O3" s="9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="AR3" s="32"/>
-      <c r="AS3" s="32"/>
-      <c r="AT3" s="32"/>
-      <c r="AU3" s="32"/>
-      <c r="AV3" s="32"/>
-      <c r="AW3" s="32"/>
-      <c r="AX3" s="32"/>
-      <c r="AY3" s="32"/>
-      <c r="AZ3" s="32"/>
-      <c r="BA3" s="32"/>
-      <c r="BB3" s="32"/>
-      <c r="BC3" s="32"/>
-      <c r="BD3" s="32"/>
-      <c r="BE3" s="32"/>
-      <c r="BF3" s="32"/>
-      <c r="BG3" s="32"/>
-      <c r="BH3" s="32"/>
-      <c r="BI3" s="32"/>
-      <c r="BJ3" s="32"/>
-      <c r="BK3" s="32"/>
-      <c r="BL3" s="32"/>
-      <c r="BM3" s="32"/>
-      <c r="BN3" s="32"/>
-      <c r="BO3" s="32"/>
-      <c r="BP3" s="32"/>
-      <c r="BQ3" s="32"/>
-      <c r="BR3" s="32"/>
-      <c r="BS3" s="32"/>
-      <c r="BT3" s="32"/>
-      <c r="BU3" s="32"/>
-      <c r="BV3" s="42"/>
-      <c r="BW3" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="BX3" s="32"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
+      <c r="AW3" s="47"/>
+      <c r="AX3" s="48"/>
+      <c r="AY3" s="37"/>
+      <c r="AZ3" s="37"/>
+      <c r="BA3" s="37"/>
+      <c r="BB3" s="37"/>
+      <c r="BC3" s="37"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="48"/>
+      <c r="BF3" s="37"/>
+      <c r="BG3" s="37"/>
+      <c r="BH3" s="37"/>
+      <c r="BI3" s="37"/>
+      <c r="BJ3" s="37"/>
+      <c r="BK3" s="47"/>
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="37"/>
+      <c r="BN3" s="37"/>
+      <c r="BO3" s="37"/>
+      <c r="BP3" s="37"/>
+      <c r="BQ3" s="37"/>
+      <c r="BR3" s="47"/>
+      <c r="BS3" s="48"/>
+      <c r="BT3" s="37"/>
+      <c r="BU3" s="37"/>
+      <c r="BV3" s="51"/>
+      <c r="BW3" s="52"/>
+      <c r="BX3" s="37"/>
       <c r="BY3" s="3"/>
       <c r="BZ3" s="3"/>
       <c r="CA3" s="3"/>
@@ -1625,40 +1756,54 @@
       <c r="CH3" s="3"/>
       <c r="CI3" s="3"/>
     </row>
-    <row r="4" s="1" customFormat="1" customHeight="1" spans="44:87">
-      <c r="AR4" s="32"/>
-      <c r="AS4" s="32"/>
-      <c r="AT4" s="32"/>
-      <c r="AU4" s="32"/>
-      <c r="AV4" s="32"/>
-      <c r="AW4" s="40"/>
-      <c r="AX4" s="41"/>
-      <c r="AY4" s="32"/>
-      <c r="AZ4" s="32"/>
-      <c r="BA4" s="32"/>
-      <c r="BB4" s="32"/>
-      <c r="BC4" s="32"/>
-      <c r="BD4" s="40"/>
-      <c r="BE4" s="41"/>
-      <c r="BF4" s="32"/>
-      <c r="BG4" s="32"/>
-      <c r="BH4" s="32"/>
-      <c r="BI4" s="32"/>
-      <c r="BJ4" s="32"/>
-      <c r="BK4" s="40"/>
-      <c r="BL4" s="41"/>
-      <c r="BM4" s="32"/>
-      <c r="BN4" s="32"/>
-      <c r="BO4" s="32"/>
-      <c r="BP4" s="32"/>
-      <c r="BQ4" s="32"/>
-      <c r="BR4" s="40"/>
-      <c r="BS4" s="41"/>
-      <c r="BT4" s="32"/>
-      <c r="BU4" s="32"/>
-      <c r="BV4" s="42"/>
-      <c r="BW4" s="43"/>
-      <c r="BX4" s="32"/>
+    <row r="4" s="1" customFormat="1" customHeight="1" spans="36:87">
+      <c r="AJ4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN4" s="27"/>
+      <c r="AO4" s="27"/>
+      <c r="AP4" s="27"/>
+      <c r="AQ4" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR4" s="9"/>
+      <c r="AS4" s="9"/>
+      <c r="AT4" s="9"/>
+      <c r="AU4" s="9"/>
+      <c r="AV4" s="9"/>
+      <c r="AW4" s="9"/>
+      <c r="AX4" s="9"/>
+      <c r="AY4" s="9"/>
+      <c r="AZ4" s="9"/>
+      <c r="BA4" s="9"/>
+      <c r="BB4" s="9"/>
+      <c r="BC4" s="9"/>
+      <c r="BD4" s="9"/>
+      <c r="BE4" s="9"/>
+      <c r="BF4" s="9"/>
+      <c r="BG4" s="9"/>
+      <c r="BH4" s="9"/>
+      <c r="BI4" s="9"/>
+      <c r="BJ4" s="9"/>
+      <c r="BK4" s="9"/>
+      <c r="BL4" s="9"/>
+      <c r="BM4" s="9"/>
+      <c r="BN4" s="9"/>
+      <c r="BO4" s="9"/>
+      <c r="BP4" s="9"/>
+      <c r="BQ4" s="9"/>
+      <c r="BR4" s="9"/>
+      <c r="BS4" s="9"/>
+      <c r="BT4" s="9"/>
+      <c r="BU4" s="9"/>
+      <c r="BV4" s="9"/>
+      <c r="BW4" s="53"/>
+      <c r="BX4" s="9"/>
       <c r="BY4" s="3"/>
       <c r="BZ4" s="3"/>
       <c r="CA4" s="3"/>
@@ -1673,7 +1818,7 @@
     </row>
     <row r="5" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B5" s="8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
@@ -1683,7 +1828,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="3"/>
       <c r="K5" s="8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -1691,19 +1836,17 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-      <c r="AJ5" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="AJ5" s="8"/>
       <c r="AK5" s="8"/>
       <c r="AL5" s="8"/>
       <c r="AM5" s="27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AN5" s="27"/>
       <c r="AO5" s="27"/>
       <c r="AP5" s="27"/>
-      <c r="AQ5" s="33" t="s">
-        <v>7</v>
+      <c r="AQ5" s="38" t="s">
+        <v>9</v>
       </c>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9"/>
@@ -1736,7 +1879,7 @@
       <c r="BT5" s="9"/>
       <c r="BU5" s="9"/>
       <c r="BV5" s="9"/>
-      <c r="BW5" s="44"/>
+      <c r="BW5" s="53"/>
       <c r="BX5" s="9"/>
       <c r="BY5" s="3"/>
       <c r="BZ5" s="3"/>
@@ -1752,7 +1895,7 @@
     </row>
     <row r="6" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B6" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1762,7 +1905,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="3"/>
       <c r="K6" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
@@ -1774,13 +1917,13 @@
       <c r="AK6" s="8"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="27" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AN6" s="27"/>
       <c r="AO6" s="27"/>
       <c r="AP6" s="27"/>
-      <c r="AQ6" s="33" t="s">
-        <v>11</v>
+      <c r="AQ6" s="38" t="s">
+        <v>13</v>
       </c>
       <c r="AR6" s="9"/>
       <c r="AS6" s="9"/>
@@ -1813,7 +1956,7 @@
       <c r="BT6" s="9"/>
       <c r="BU6" s="9"/>
       <c r="BV6" s="9"/>
-      <c r="BW6" s="44"/>
+      <c r="BW6" s="53"/>
       <c r="BX6" s="9"/>
       <c r="BY6" s="3"/>
       <c r="BZ6" s="3"/>
@@ -1829,7 +1972,7 @@
     </row>
     <row r="7" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B7" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -1839,7 +1982,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="3"/>
       <c r="K7" s="22" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
@@ -1851,13 +1994,13 @@
       <c r="AK7" s="8"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="27" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AN7" s="27"/>
       <c r="AO7" s="27"/>
       <c r="AP7" s="27"/>
-      <c r="AQ7" s="33" t="s">
-        <v>15</v>
+      <c r="AQ7" s="38" t="s">
+        <v>17</v>
       </c>
       <c r="AR7" s="9"/>
       <c r="AS7" s="9"/>
@@ -1890,7 +2033,7 @@
       <c r="BT7" s="9"/>
       <c r="BU7" s="9"/>
       <c r="BV7" s="9"/>
-      <c r="BW7" s="44"/>
+      <c r="BW7" s="53"/>
       <c r="BX7" s="9"/>
       <c r="BY7" s="3"/>
       <c r="BZ7" s="3"/>
@@ -1906,7 +2049,7 @@
     </row>
     <row r="8" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B8" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1922,51 +2065,51 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AN8" s="27"/>
-      <c r="AO8" s="27"/>
-      <c r="AP8" s="27"/>
-      <c r="AQ8" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR8" s="9"/>
-      <c r="AS8" s="9"/>
-      <c r="AT8" s="9"/>
-      <c r="AU8" s="9"/>
-      <c r="AV8" s="9"/>
-      <c r="AW8" s="9"/>
-      <c r="AX8" s="9"/>
-      <c r="AY8" s="9"/>
-      <c r="AZ8" s="9"/>
-      <c r="BA8" s="9"/>
-      <c r="BB8" s="9"/>
-      <c r="BC8" s="9"/>
-      <c r="BD8" s="9"/>
-      <c r="BE8" s="9"/>
-      <c r="BF8" s="9"/>
-      <c r="BG8" s="9"/>
-      <c r="BH8" s="9"/>
-      <c r="BI8" s="9"/>
-      <c r="BJ8" s="9"/>
-      <c r="BK8" s="9"/>
-      <c r="BL8" s="9"/>
-      <c r="BM8" s="9"/>
-      <c r="BN8" s="9"/>
-      <c r="BO8" s="9"/>
-      <c r="BP8" s="9"/>
-      <c r="BQ8" s="9"/>
-      <c r="BR8" s="9"/>
-      <c r="BS8" s="9"/>
-      <c r="BT8" s="9"/>
-      <c r="BU8" s="9"/>
-      <c r="BV8" s="9"/>
-      <c r="BW8" s="44"/>
-      <c r="BX8" s="9"/>
+      <c r="AJ8" s="28"/>
+      <c r="AK8" s="28"/>
+      <c r="AL8" s="28"/>
+      <c r="AM8" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN8" s="29"/>
+      <c r="AO8" s="29"/>
+      <c r="AP8" s="29"/>
+      <c r="AQ8" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
+      <c r="AT8" s="20"/>
+      <c r="AU8" s="20"/>
+      <c r="AV8" s="20"/>
+      <c r="AW8" s="20"/>
+      <c r="AX8" s="20"/>
+      <c r="AY8" s="20"/>
+      <c r="AZ8" s="20"/>
+      <c r="BA8" s="20"/>
+      <c r="BB8" s="20"/>
+      <c r="BC8" s="20"/>
+      <c r="BD8" s="20"/>
+      <c r="BE8" s="20"/>
+      <c r="BF8" s="20"/>
+      <c r="BG8" s="20"/>
+      <c r="BH8" s="20"/>
+      <c r="BI8" s="20"/>
+      <c r="BJ8" s="20"/>
+      <c r="BK8" s="20"/>
+      <c r="BL8" s="20"/>
+      <c r="BM8" s="20"/>
+      <c r="BN8" s="20"/>
+      <c r="BO8" s="20"/>
+      <c r="BP8" s="20"/>
+      <c r="BQ8" s="20"/>
+      <c r="BR8" s="20"/>
+      <c r="BS8" s="20"/>
+      <c r="BT8" s="20"/>
+      <c r="BU8" s="20"/>
+      <c r="BV8" s="20"/>
+      <c r="BW8" s="54"/>
+      <c r="BX8" s="20"/>
       <c r="BY8" s="3"/>
       <c r="BZ8" s="3"/>
       <c r="CA8" s="3"/>
@@ -1981,7 +2124,7 @@
     </row>
     <row r="9" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -1991,7 +2134,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="3"/>
       <c r="K9" s="22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1999,51 +2142,53 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="AJ9" s="28"/>
-      <c r="AK9" s="28"/>
-      <c r="AL9" s="28"/>
-      <c r="AM9" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN9" s="29"/>
-      <c r="AO9" s="29"/>
-      <c r="AP9" s="29"/>
-      <c r="AQ9" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR9" s="20"/>
-      <c r="AS9" s="20"/>
-      <c r="AT9" s="20"/>
-      <c r="AU9" s="20"/>
-      <c r="AV9" s="20"/>
-      <c r="AW9" s="20"/>
-      <c r="AX9" s="20"/>
-      <c r="AY9" s="20"/>
-      <c r="AZ9" s="20"/>
-      <c r="BA9" s="20"/>
-      <c r="BB9" s="20"/>
-      <c r="BC9" s="20"/>
-      <c r="BD9" s="20"/>
-      <c r="BE9" s="20"/>
-      <c r="BF9" s="20"/>
-      <c r="BG9" s="20"/>
-      <c r="BH9" s="20"/>
-      <c r="BI9" s="20"/>
-      <c r="BJ9" s="20"/>
-      <c r="BK9" s="20"/>
-      <c r="BL9" s="20"/>
-      <c r="BM9" s="20"/>
-      <c r="BN9" s="20"/>
-      <c r="BO9" s="20"/>
-      <c r="BP9" s="20"/>
-      <c r="BQ9" s="20"/>
-      <c r="BR9" s="20"/>
-      <c r="BS9" s="20"/>
-      <c r="BT9" s="20"/>
-      <c r="BU9" s="20"/>
-      <c r="BV9" s="20"/>
-      <c r="BW9" s="45"/>
-      <c r="BX9" s="20"/>
+      <c r="AJ9" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK9" s="31"/>
+      <c r="AL9" s="31"/>
+      <c r="AM9" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="AN9" s="32"/>
+      <c r="AO9" s="32"/>
+      <c r="AP9" s="32"/>
+      <c r="AQ9" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR9" s="41"/>
+      <c r="AS9" s="41"/>
+      <c r="AT9" s="41"/>
+      <c r="AU9" s="41"/>
+      <c r="AV9" s="41"/>
+      <c r="AW9" s="41"/>
+      <c r="AX9" s="41"/>
+      <c r="AY9" s="41"/>
+      <c r="AZ9" s="41"/>
+      <c r="BA9" s="41"/>
+      <c r="BB9" s="41"/>
+      <c r="BC9" s="41"/>
+      <c r="BD9" s="41"/>
+      <c r="BE9" s="41"/>
+      <c r="BF9" s="41"/>
+      <c r="BG9" s="41"/>
+      <c r="BH9" s="41"/>
+      <c r="BI9" s="41"/>
+      <c r="BJ9" s="41"/>
+      <c r="BK9" s="41"/>
+      <c r="BL9" s="41"/>
+      <c r="BM9" s="41"/>
+      <c r="BN9" s="41"/>
+      <c r="BO9" s="41"/>
+      <c r="BP9" s="41"/>
+      <c r="BQ9" s="41"/>
+      <c r="BR9" s="41"/>
+      <c r="BS9" s="41"/>
+      <c r="BT9" s="41"/>
+      <c r="BU9" s="41"/>
+      <c r="BV9" s="41"/>
+      <c r="BW9" s="55"/>
+      <c r="BX9" s="41"/>
       <c r="BY9" s="3"/>
       <c r="BZ9" s="3"/>
       <c r="CA9" s="3"/>
@@ -2058,7 +2203,7 @@
     </row>
     <row r="10" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B10" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -2074,53 +2219,51 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="AJ10" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="AK10" s="30"/>
-      <c r="AL10" s="30"/>
-      <c r="AM10" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN10" s="31"/>
-      <c r="AO10" s="31"/>
-      <c r="AP10" s="31"/>
-      <c r="AQ10" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="AR10" s="36"/>
-      <c r="AS10" s="36"/>
-      <c r="AT10" s="36"/>
-      <c r="AU10" s="36"/>
-      <c r="AV10" s="36"/>
-      <c r="AW10" s="36"/>
-      <c r="AX10" s="36"/>
-      <c r="AY10" s="36"/>
-      <c r="AZ10" s="36"/>
-      <c r="BA10" s="36"/>
-      <c r="BB10" s="36"/>
-      <c r="BC10" s="36"/>
-      <c r="BD10" s="36"/>
-      <c r="BE10" s="36"/>
-      <c r="BF10" s="36"/>
-      <c r="BG10" s="36"/>
-      <c r="BH10" s="36"/>
-      <c r="BI10" s="36"/>
-      <c r="BJ10" s="36"/>
-      <c r="BK10" s="36"/>
-      <c r="BL10" s="36"/>
-      <c r="BM10" s="36"/>
-      <c r="BN10" s="36"/>
-      <c r="BO10" s="36"/>
-      <c r="BP10" s="36"/>
-      <c r="BQ10" s="36"/>
-      <c r="BR10" s="36"/>
-      <c r="BS10" s="36"/>
-      <c r="BT10" s="36"/>
-      <c r="BU10" s="36"/>
-      <c r="BV10" s="36"/>
-      <c r="BW10" s="46"/>
-      <c r="BX10" s="36"/>
+      <c r="AJ10" s="33"/>
+      <c r="AK10" s="34"/>
+      <c r="AL10" s="34"/>
+      <c r="AM10" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="AN10" s="27"/>
+      <c r="AO10" s="27"/>
+      <c r="AP10" s="27"/>
+      <c r="AQ10" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR10" s="9"/>
+      <c r="AS10" s="9"/>
+      <c r="AT10" s="9"/>
+      <c r="AU10" s="9"/>
+      <c r="AV10" s="9"/>
+      <c r="AW10" s="9"/>
+      <c r="AX10" s="9"/>
+      <c r="AY10" s="9"/>
+      <c r="AZ10" s="9"/>
+      <c r="BA10" s="9"/>
+      <c r="BB10" s="9"/>
+      <c r="BC10" s="9"/>
+      <c r="BD10" s="9"/>
+      <c r="BE10" s="9"/>
+      <c r="BF10" s="9"/>
+      <c r="BG10" s="9"/>
+      <c r="BH10" s="9"/>
+      <c r="BI10" s="9"/>
+      <c r="BJ10" s="9"/>
+      <c r="BK10" s="9"/>
+      <c r="BL10" s="9"/>
+      <c r="BM10" s="9"/>
+      <c r="BN10" s="9"/>
+      <c r="BO10" s="9"/>
+      <c r="BP10" s="9"/>
+      <c r="BQ10" s="9"/>
+      <c r="BR10" s="9"/>
+      <c r="BS10" s="9"/>
+      <c r="BT10" s="9"/>
+      <c r="BU10" s="9"/>
+      <c r="BV10" s="9"/>
+      <c r="BW10" s="53"/>
+      <c r="BX10" s="9"/>
       <c r="BY10" s="3"/>
       <c r="BZ10" s="3"/>
       <c r="CA10" s="3"/>
@@ -2149,17 +2292,17 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="AJ11" s="8"/>
-      <c r="AK11" s="8"/>
-      <c r="AL11" s="8"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="34"/>
+      <c r="AL11" s="34"/>
       <c r="AM11" s="27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AN11" s="27"/>
       <c r="AO11" s="27"/>
       <c r="AP11" s="27"/>
-      <c r="AQ11" s="33" t="s">
-        <v>28</v>
+      <c r="AQ11" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="AR11" s="9"/>
       <c r="AS11" s="9"/>
@@ -2192,7 +2335,7 @@
       <c r="BT11" s="9"/>
       <c r="BU11" s="9"/>
       <c r="BV11" s="9"/>
-      <c r="BW11" s="44"/>
+      <c r="BW11" s="53"/>
       <c r="BX11" s="9"/>
       <c r="BY11" s="3"/>
       <c r="BZ11" s="3"/>
@@ -2222,17 +2365,17 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="AJ12" s="8"/>
-      <c r="AK12" s="8"/>
-      <c r="AL12" s="8"/>
+      <c r="AJ12" s="33"/>
+      <c r="AK12" s="34"/>
+      <c r="AL12" s="34"/>
       <c r="AM12" s="27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AN12" s="27"/>
       <c r="AO12" s="27"/>
       <c r="AP12" s="27"/>
-      <c r="AQ12" s="33" t="s">
-        <v>30</v>
+      <c r="AQ12" s="38" t="s">
+        <v>32</v>
       </c>
       <c r="AR12" s="9"/>
       <c r="AS12" s="9"/>
@@ -2265,7 +2408,7 @@
       <c r="BT12" s="9"/>
       <c r="BU12" s="9"/>
       <c r="BV12" s="9"/>
-      <c r="BW12" s="44"/>
+      <c r="BW12" s="53"/>
       <c r="BX12" s="9"/>
       <c r="BY12" s="3"/>
       <c r="BZ12" s="3"/>
@@ -2295,17 +2438,17 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="AJ13" s="8"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="8"/>
+      <c r="AJ13" s="33"/>
+      <c r="AK13" s="34"/>
+      <c r="AL13" s="34"/>
       <c r="AM13" s="27" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AN13" s="27"/>
       <c r="AO13" s="27"/>
       <c r="AP13" s="27"/>
-      <c r="AQ13" s="33" t="s">
-        <v>32</v>
+      <c r="AQ13" s="38" t="s">
+        <v>34</v>
       </c>
       <c r="AR13" s="9"/>
       <c r="AS13" s="9"/>
@@ -2338,7 +2481,7 @@
       <c r="BT13" s="9"/>
       <c r="BU13" s="9"/>
       <c r="BV13" s="9"/>
-      <c r="BW13" s="44"/>
+      <c r="BW13" s="53"/>
       <c r="BX13" s="9"/>
       <c r="BY13" s="3"/>
       <c r="BZ13" s="3"/>
@@ -2368,17 +2511,17 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
+      <c r="AJ14" s="33"/>
+      <c r="AK14" s="34"/>
+      <c r="AL14" s="34"/>
       <c r="AM14" s="27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AN14" s="27"/>
       <c r="AO14" s="27"/>
       <c r="AP14" s="27"/>
-      <c r="AQ14" s="33" t="s">
-        <v>34</v>
+      <c r="AQ14" s="38" t="s">
+        <v>36</v>
       </c>
       <c r="AR14" s="9"/>
       <c r="AS14" s="9"/>
@@ -2411,7 +2554,7 @@
       <c r="BT14" s="9"/>
       <c r="BU14" s="9"/>
       <c r="BV14" s="9"/>
-      <c r="BW14" s="44"/>
+      <c r="BW14" s="53"/>
       <c r="BX14" s="9"/>
       <c r="BY14" s="3"/>
       <c r="BZ14" s="3"/>
@@ -2441,17 +2584,17 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="AJ15" s="8"/>
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="8"/>
+      <c r="AJ15" s="35"/>
+      <c r="AK15" s="36"/>
+      <c r="AL15" s="36"/>
       <c r="AM15" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AN15" s="27"/>
       <c r="AO15" s="27"/>
       <c r="AP15" s="27"/>
-      <c r="AQ15" s="33" t="s">
-        <v>36</v>
+      <c r="AQ15" s="38" t="s">
+        <v>38</v>
       </c>
       <c r="AR15" s="9"/>
       <c r="AS15" s="9"/>
@@ -2484,7 +2627,7 @@
       <c r="BT15" s="9"/>
       <c r="BU15" s="9"/>
       <c r="BV15" s="9"/>
-      <c r="BW15" s="44"/>
+      <c r="BW15" s="53"/>
       <c r="BX15" s="9"/>
       <c r="BY15" s="3"/>
       <c r="BZ15" s="3"/>
@@ -2528,169 +2671,172 @@
       <c r="CH16" s="3"/>
       <c r="CI16" s="3"/>
     </row>
-    <row r="17" s="1" customFormat="1" customHeight="1" spans="44:87">
-      <c r="AR17" s="32">
+    <row r="17" s="1" customFormat="1" customHeight="1" spans="44:88">
+      <c r="AR17" s="37">
         <v>1</v>
       </c>
-      <c r="AS17" s="32">
+      <c r="AS17" s="37">
         <v>2</v>
       </c>
-      <c r="AT17" s="32">
+      <c r="AT17" s="37">
         <v>3</v>
       </c>
-      <c r="AU17" s="32">
+      <c r="AU17" s="37">
         <v>4</v>
       </c>
-      <c r="AV17" s="32">
+      <c r="AV17" s="37">
         <v>5</v>
       </c>
-      <c r="AW17" s="32">
+      <c r="AW17" s="37">
         <v>6</v>
       </c>
-      <c r="AX17" s="32">
+      <c r="AX17" s="37">
         <v>7</v>
       </c>
-      <c r="AY17" s="32">
+      <c r="AY17" s="37">
         <v>8</v>
       </c>
-      <c r="AZ17" s="32">
+      <c r="AZ17" s="37">
         <v>9</v>
       </c>
-      <c r="BA17" s="32">
+      <c r="BA17" s="37">
         <v>10</v>
       </c>
-      <c r="BB17" s="32">
+      <c r="BB17" s="37">
         <v>11</v>
       </c>
-      <c r="BC17" s="32">
+      <c r="BC17" s="37">
         <v>12</v>
       </c>
-      <c r="BD17" s="32">
+      <c r="BD17" s="37">
         <v>13</v>
       </c>
-      <c r="BE17" s="32">
+      <c r="BE17" s="37">
         <v>14</v>
       </c>
-      <c r="BF17" s="32">
+      <c r="BF17" s="37">
         <v>15</v>
       </c>
-      <c r="BG17" s="32">
+      <c r="BG17" s="37">
         <v>16</v>
       </c>
-      <c r="BH17" s="32">
+      <c r="BH17" s="37">
         <v>17</v>
       </c>
-      <c r="BI17" s="32">
+      <c r="BI17" s="37">
         <v>18</v>
       </c>
-      <c r="BJ17" s="32">
+      <c r="BJ17" s="37">
         <v>19</v>
       </c>
-      <c r="BK17" s="32">
+      <c r="BK17" s="37">
         <v>20</v>
       </c>
-      <c r="BL17" s="32">
+      <c r="BL17" s="37">
         <v>21</v>
       </c>
-      <c r="BM17" s="32">
+      <c r="BM17" s="37">
         <v>22</v>
       </c>
-      <c r="BN17" s="32">
+      <c r="BN17" s="37">
         <v>23</v>
       </c>
-      <c r="BO17" s="32">
+      <c r="BO17" s="37">
         <v>24</v>
       </c>
-      <c r="BP17" s="32">
+      <c r="BP17" s="37">
         <v>25</v>
       </c>
-      <c r="BQ17" s="32">
+      <c r="BQ17" s="37">
         <v>26</v>
       </c>
-      <c r="BR17" s="32">
+      <c r="BR17" s="37">
         <v>27</v>
       </c>
-      <c r="BS17" s="32">
+      <c r="BS17" s="37">
         <v>28</v>
       </c>
-      <c r="BT17" s="32">
+      <c r="BT17" s="37">
         <v>29</v>
       </c>
-      <c r="BU17" s="32">
+      <c r="BU17" s="37">
         <v>30</v>
       </c>
-      <c r="BV17" s="42">
+      <c r="BV17" s="51">
         <v>31</v>
       </c>
-      <c r="BW17" s="47" t="s">
+      <c r="BW17" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="BX17" s="57"/>
+      <c r="BY17" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="BZ17" s="57"/>
+      <c r="CA17" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="CB17" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="CC17" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="CD17" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="CE17" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="CF17" s="59" t="s">
+        <v>35</v>
+      </c>
+      <c r="CG17" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="BX17" s="48"/>
-      <c r="BY17" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="BZ17" s="48"/>
-      <c r="CA17" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="CB17" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="CC17" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="CD17" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="CE17" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="CF17" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="CG17" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="CH17" s="48"/>
-      <c r="CI17" s="48"/>
-    </row>
-    <row r="18" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CH17" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="CI17" s="68"/>
+      <c r="CJ17" s="68"/>
+    </row>
+    <row r="18" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B18" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11"/>
       <c r="K18" s="12"/>
       <c r="L18" s="10" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
       <c r="S18" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
       <c r="X18" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="10"/>
@@ -2698,135 +2844,136 @@
       <c r="AB18" s="10"/>
       <c r="AC18" s="10"/>
       <c r="AD18" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AE18" s="10"/>
       <c r="AF18" s="10"/>
       <c r="AG18" s="10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH18" s="10"/>
       <c r="AI18" s="10"/>
       <c r="AJ18" s="10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK18" s="10"/>
       <c r="AL18" s="10"/>
       <c r="AM18" s="10"/>
       <c r="AN18" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AO18" s="10"/>
       <c r="AP18" s="10"/>
-      <c r="AQ18" s="37"/>
-      <c r="AR18" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS18" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="AT18" s="32" t="s">
+      <c r="AQ18" s="42"/>
+      <c r="AR18" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="AU18" s="32" t="s">
+      <c r="AS18" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="AV18" s="32" t="s">
+      <c r="AT18" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="AW18" s="40" t="s">
+      <c r="AU18" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="AX18" s="41" t="s">
+      <c r="AV18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="AY18" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="AZ18" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="BA18" s="32" t="s">
+      <c r="AW18" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX18" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY18" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="BB18" s="32" t="s">
+      <c r="AZ18" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="BC18" s="32" t="s">
+      <c r="BA18" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="BD18" s="40" t="s">
+      <c r="BB18" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="BE18" s="41" t="s">
+      <c r="BC18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BF18" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="BG18" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="BH18" s="32" t="s">
+      <c r="BD18" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="BE18" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="BF18" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="BI18" s="32" t="s">
+      <c r="BG18" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="BJ18" s="32" t="s">
+      <c r="BH18" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="BK18" s="40" t="s">
+      <c r="BI18" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="BL18" s="41" t="s">
+      <c r="BJ18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BM18" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="BN18" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="BO18" s="32" t="s">
+      <c r="BK18" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL18" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM18" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="BP18" s="32" t="s">
+      <c r="BN18" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="BQ18" s="32" t="s">
+      <c r="BO18" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="BR18" s="40" t="s">
+      <c r="BP18" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="BS18" s="41" t="s">
+      <c r="BQ18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BT18" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="BU18" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="BV18" s="42" t="s">
+      <c r="BR18" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="BS18" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="BT18" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="BW18" s="51"/>
-      <c r="BX18" s="48"/>
-      <c r="BY18" s="48"/>
-      <c r="BZ18" s="48"/>
-      <c r="CA18" s="50"/>
-      <c r="CB18" s="50"/>
-      <c r="CC18" s="50"/>
-      <c r="CD18" s="50"/>
-      <c r="CE18" s="50"/>
-      <c r="CF18" s="50"/>
-      <c r="CG18" s="48"/>
-      <c r="CH18" s="48"/>
-      <c r="CI18" s="48"/>
-    </row>
-    <row r="19" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="BU18" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="BV18" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="BW18" s="61"/>
+      <c r="BX18" s="62"/>
+      <c r="BY18" s="62"/>
+      <c r="BZ18" s="62"/>
+      <c r="CA18" s="63"/>
+      <c r="CB18" s="63"/>
+      <c r="CC18" s="63"/>
+      <c r="CD18" s="63"/>
+      <c r="CE18" s="63"/>
+      <c r="CF18" s="63"/>
+      <c r="CG18" s="63"/>
+      <c r="CH18" s="68"/>
+      <c r="CI18" s="68"/>
+      <c r="CJ18" s="68"/>
+    </row>
+    <row r="19" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B19" s="14"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
@@ -2867,54 +3014,55 @@
       <c r="AM19" s="15"/>
       <c r="AN19" s="15"/>
       <c r="AO19" s="15"/>
-      <c r="AP19" s="38"/>
+      <c r="AP19" s="44"/>
       <c r="AQ19" s="3"/>
-      <c r="AR19" s="14"/>
-      <c r="AS19" s="15"/>
-      <c r="AT19" s="15"/>
-      <c r="AU19" s="15"/>
-      <c r="AV19" s="15"/>
-      <c r="AW19" s="15"/>
-      <c r="AX19" s="15"/>
-      <c r="AY19" s="15"/>
-      <c r="AZ19" s="15"/>
-      <c r="BA19" s="15"/>
-      <c r="BB19" s="15"/>
-      <c r="BC19" s="15"/>
-      <c r="BD19" s="15"/>
-      <c r="BE19" s="15"/>
-      <c r="BF19" s="15"/>
-      <c r="BG19" s="15"/>
-      <c r="BH19" s="15"/>
-      <c r="BI19" s="15"/>
-      <c r="BJ19" s="15"/>
-      <c r="BK19" s="15"/>
-      <c r="BL19" s="15"/>
-      <c r="BM19" s="15"/>
-      <c r="BN19" s="15"/>
-      <c r="BO19" s="15"/>
-      <c r="BP19" s="15"/>
-      <c r="BQ19" s="15"/>
-      <c r="BR19" s="15"/>
-      <c r="BS19" s="15"/>
-      <c r="BT19" s="15"/>
-      <c r="BU19" s="15"/>
-      <c r="BV19" s="15"/>
-      <c r="BW19" s="52"/>
-      <c r="BX19" s="52"/>
-      <c r="BY19" s="52"/>
-      <c r="BZ19" s="52"/>
-      <c r="CA19" s="52"/>
-      <c r="CB19" s="52"/>
-      <c r="CC19" s="52"/>
-      <c r="CD19" s="52"/>
-      <c r="CE19" s="52"/>
-      <c r="CF19" s="52"/>
-      <c r="CG19" s="52"/>
-      <c r="CH19" s="52"/>
-      <c r="CI19" s="57"/>
-    </row>
-    <row r="20" s="2" customFormat="1" customHeight="1" spans="2:87">
+      <c r="AR19" s="45"/>
+      <c r="AS19" s="45"/>
+      <c r="AT19" s="45"/>
+      <c r="AU19" s="45"/>
+      <c r="AV19" s="45"/>
+      <c r="AW19" s="45"/>
+      <c r="AX19" s="45"/>
+      <c r="AY19" s="45"/>
+      <c r="AZ19" s="45"/>
+      <c r="BA19" s="45"/>
+      <c r="BB19" s="45"/>
+      <c r="BC19" s="45"/>
+      <c r="BD19" s="45"/>
+      <c r="BE19" s="45"/>
+      <c r="BF19" s="45"/>
+      <c r="BG19" s="45"/>
+      <c r="BH19" s="45"/>
+      <c r="BI19" s="45"/>
+      <c r="BJ19" s="45"/>
+      <c r="BK19" s="45"/>
+      <c r="BL19" s="45"/>
+      <c r="BM19" s="45"/>
+      <c r="BN19" s="45"/>
+      <c r="BO19" s="45"/>
+      <c r="BP19" s="45"/>
+      <c r="BQ19" s="45"/>
+      <c r="BR19" s="45"/>
+      <c r="BS19" s="45"/>
+      <c r="BT19" s="45"/>
+      <c r="BU19" s="45"/>
+      <c r="BV19" s="45"/>
+      <c r="BW19" s="45"/>
+      <c r="BX19" s="45"/>
+      <c r="BY19" s="45"/>
+      <c r="BZ19" s="45"/>
+      <c r="CA19" s="45"/>
+      <c r="CB19" s="45"/>
+      <c r="CC19" s="45"/>
+      <c r="CD19" s="45"/>
+      <c r="CE19" s="45"/>
+      <c r="CF19" s="45"/>
+      <c r="CG19" s="45"/>
+      <c r="CH19" s="45"/>
+      <c r="CI19" s="45"/>
+      <c r="CJ19" s="45"/>
+    </row>
+    <row r="20" s="2" customFormat="1" customHeight="1" spans="2:88">
       <c r="B20" s="16">
         <v>1</v>
       </c>
@@ -2988,8 +3136,8 @@
       <c r="BS20" s="18"/>
       <c r="BT20" s="18"/>
       <c r="BU20" s="18"/>
-      <c r="BV20" s="53"/>
-      <c r="BW20" s="54"/>
+      <c r="BV20" s="64"/>
+      <c r="BW20" s="65"/>
       <c r="BX20" s="18"/>
       <c r="BY20" s="18"/>
       <c r="BZ20" s="18"/>
@@ -2999,11 +3147,12 @@
       <c r="CD20" s="18"/>
       <c r="CE20" s="18"/>
       <c r="CF20" s="18"/>
-      <c r="CG20" s="18"/>
-      <c r="CH20" s="18"/>
-      <c r="CI20" s="18"/>
-    </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG20" s="16"/>
+      <c r="CH20" s="69"/>
+      <c r="CI20" s="70"/>
+      <c r="CJ20" s="71"/>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B21" s="19">
         <v>2</v>
       </c>
@@ -3078,7 +3227,7 @@
       <c r="BT21" s="9"/>
       <c r="BU21" s="9"/>
       <c r="BV21" s="6"/>
-      <c r="BW21" s="44"/>
+      <c r="BW21" s="53"/>
       <c r="BX21" s="9"/>
       <c r="BY21" s="9"/>
       <c r="BZ21" s="9"/>
@@ -3088,11 +3237,12 @@
       <c r="CD21" s="9"/>
       <c r="CE21" s="9"/>
       <c r="CF21" s="9"/>
-      <c r="CG21" s="9"/>
-      <c r="CH21" s="9"/>
-      <c r="CI21" s="9"/>
-    </row>
-    <row r="22" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG21" s="19"/>
+      <c r="CH21" s="69"/>
+      <c r="CI21" s="70"/>
+      <c r="CJ21" s="71"/>
+    </row>
+    <row r="22" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B22" s="19">
         <v>3</v>
       </c>
@@ -3167,7 +3317,7 @@
       <c r="BT22" s="9"/>
       <c r="BU22" s="9"/>
       <c r="BV22" s="6"/>
-      <c r="BW22" s="44"/>
+      <c r="BW22" s="53"/>
       <c r="BX22" s="9"/>
       <c r="BY22" s="9"/>
       <c r="BZ22" s="9"/>
@@ -3177,11 +3327,12 @@
       <c r="CD22" s="9"/>
       <c r="CE22" s="9"/>
       <c r="CF22" s="9"/>
-      <c r="CG22" s="9"/>
-      <c r="CH22" s="9"/>
-      <c r="CI22" s="9"/>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG22" s="19"/>
+      <c r="CH22" s="69"/>
+      <c r="CI22" s="70"/>
+      <c r="CJ22" s="71"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B23" s="19">
         <v>4</v>
       </c>
@@ -3256,7 +3407,7 @@
       <c r="BT23" s="9"/>
       <c r="BU23" s="9"/>
       <c r="BV23" s="6"/>
-      <c r="BW23" s="44"/>
+      <c r="BW23" s="53"/>
       <c r="BX23" s="9"/>
       <c r="BY23" s="9"/>
       <c r="BZ23" s="9"/>
@@ -3266,11 +3417,12 @@
       <c r="CD23" s="9"/>
       <c r="CE23" s="9"/>
       <c r="CF23" s="9"/>
-      <c r="CG23" s="9"/>
-      <c r="CH23" s="9"/>
-      <c r="CI23" s="9"/>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG23" s="19"/>
+      <c r="CH23" s="69"/>
+      <c r="CI23" s="70"/>
+      <c r="CJ23" s="71"/>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B24" s="19">
         <v>5</v>
       </c>
@@ -3345,7 +3497,7 @@
       <c r="BT24" s="9"/>
       <c r="BU24" s="9"/>
       <c r="BV24" s="6"/>
-      <c r="BW24" s="44"/>
+      <c r="BW24" s="53"/>
       <c r="BX24" s="9"/>
       <c r="BY24" s="9"/>
       <c r="BZ24" s="9"/>
@@ -3355,11 +3507,12 @@
       <c r="CD24" s="9"/>
       <c r="CE24" s="9"/>
       <c r="CF24" s="9"/>
-      <c r="CG24" s="9"/>
-      <c r="CH24" s="9"/>
-      <c r="CI24" s="9"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG24" s="19"/>
+      <c r="CH24" s="69"/>
+      <c r="CI24" s="70"/>
+      <c r="CJ24" s="71"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B25" s="19">
         <v>6</v>
       </c>
@@ -3434,7 +3587,7 @@
       <c r="BT25" s="9"/>
       <c r="BU25" s="9"/>
       <c r="BV25" s="6"/>
-      <c r="BW25" s="44"/>
+      <c r="BW25" s="53"/>
       <c r="BX25" s="9"/>
       <c r="BY25" s="9"/>
       <c r="BZ25" s="9"/>
@@ -3444,11 +3597,12 @@
       <c r="CD25" s="9"/>
       <c r="CE25" s="9"/>
       <c r="CF25" s="9"/>
-      <c r="CG25" s="9"/>
-      <c r="CH25" s="9"/>
-      <c r="CI25" s="9"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG25" s="19"/>
+      <c r="CH25" s="69"/>
+      <c r="CI25" s="70"/>
+      <c r="CJ25" s="71"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B26" s="19">
         <v>7</v>
       </c>
@@ -3523,7 +3677,7 @@
       <c r="BT26" s="9"/>
       <c r="BU26" s="9"/>
       <c r="BV26" s="6"/>
-      <c r="BW26" s="44"/>
+      <c r="BW26" s="53"/>
       <c r="BX26" s="9"/>
       <c r="BY26" s="9"/>
       <c r="BZ26" s="9"/>
@@ -3533,11 +3687,12 @@
       <c r="CD26" s="9"/>
       <c r="CE26" s="9"/>
       <c r="CF26" s="9"/>
-      <c r="CG26" s="9"/>
-      <c r="CH26" s="9"/>
-      <c r="CI26" s="9"/>
-    </row>
-    <row r="27" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG26" s="19"/>
+      <c r="CH26" s="69"/>
+      <c r="CI26" s="70"/>
+      <c r="CJ26" s="71"/>
+    </row>
+    <row r="27" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B27" s="19">
         <v>8</v>
       </c>
@@ -3612,7 +3767,7 @@
       <c r="BT27" s="9"/>
       <c r="BU27" s="9"/>
       <c r="BV27" s="6"/>
-      <c r="BW27" s="44"/>
+      <c r="BW27" s="53"/>
       <c r="BX27" s="9"/>
       <c r="BY27" s="9"/>
       <c r="BZ27" s="9"/>
@@ -3622,11 +3777,12 @@
       <c r="CD27" s="9"/>
       <c r="CE27" s="9"/>
       <c r="CF27" s="9"/>
-      <c r="CG27" s="9"/>
-      <c r="CH27" s="9"/>
-      <c r="CI27" s="9"/>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG27" s="19"/>
+      <c r="CH27" s="69"/>
+      <c r="CI27" s="70"/>
+      <c r="CJ27" s="71"/>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B28" s="19">
         <v>9</v>
       </c>
@@ -3700,8 +3856,8 @@
       <c r="BS28" s="20"/>
       <c r="BT28" s="20"/>
       <c r="BU28" s="20"/>
-      <c r="BV28" s="55"/>
-      <c r="BW28" s="45"/>
+      <c r="BV28" s="66"/>
+      <c r="BW28" s="54"/>
       <c r="BX28" s="20"/>
       <c r="BY28" s="20"/>
       <c r="BZ28" s="20"/>
@@ -3711,11 +3867,12 @@
       <c r="CD28" s="20"/>
       <c r="CE28" s="20"/>
       <c r="CF28" s="20"/>
-      <c r="CG28" s="20"/>
-      <c r="CH28" s="20"/>
-      <c r="CI28" s="20"/>
-    </row>
-    <row r="29" s="1" customFormat="1" customHeight="1" spans="2:87">
+      <c r="CG28" s="72"/>
+      <c r="CH28" s="69"/>
+      <c r="CI28" s="70"/>
+      <c r="CJ28" s="71"/>
+    </row>
+    <row r="29" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B29" s="19">
         <v>10</v>
       </c>
@@ -3759,7 +3916,7 @@
       <c r="AN29" s="9"/>
       <c r="AO29" s="9"/>
       <c r="AP29" s="9"/>
-      <c r="AQ29" s="39"/>
+      <c r="AQ29" s="46"/>
       <c r="AR29" s="9"/>
       <c r="AS29" s="9"/>
       <c r="AT29" s="9"/>
@@ -3801,9 +3958,10 @@
       <c r="CD29" s="9"/>
       <c r="CE29" s="9"/>
       <c r="CF29" s="9"/>
-      <c r="CG29" s="9"/>
-      <c r="CH29" s="9"/>
-      <c r="CI29" s="9"/>
+      <c r="CG29" s="19"/>
+      <c r="CH29" s="69"/>
+      <c r="CI29" s="70"/>
+      <c r="CJ29" s="71"/>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B30" s="3"/>
@@ -3841,14 +3999,14 @@
       <c r="BY30" s="3"/>
       <c r="BZ30" s="3"/>
       <c r="CA30" s="3"/>
-      <c r="CB30" s="56"/>
-      <c r="CC30" s="56"/>
-      <c r="CD30" s="56"/>
-      <c r="CE30" s="56"/>
-      <c r="CF30" s="56"/>
-      <c r="CG30" s="56"/>
-      <c r="CH30" s="56"/>
-      <c r="CI30" s="56"/>
+      <c r="CB30" s="67"/>
+      <c r="CC30" s="67"/>
+      <c r="CD30" s="67"/>
+      <c r="CE30" s="67"/>
+      <c r="CF30" s="67"/>
+      <c r="CG30" s="67"/>
+      <c r="CH30" s="67"/>
+      <c r="CI30" s="67"/>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B31" s="3"/>
@@ -3886,14 +4044,14 @@
       <c r="BY31" s="3"/>
       <c r="BZ31" s="3"/>
       <c r="CA31" s="3"/>
-      <c r="CB31" s="56"/>
-      <c r="CC31" s="56"/>
-      <c r="CD31" s="56"/>
-      <c r="CE31" s="56"/>
-      <c r="CF31" s="56"/>
-      <c r="CG31" s="56"/>
-      <c r="CH31" s="56"/>
-      <c r="CI31" s="56"/>
+      <c r="CB31" s="67"/>
+      <c r="CC31" s="67"/>
+      <c r="CD31" s="67"/>
+      <c r="CE31" s="67"/>
+      <c r="CF31" s="67"/>
+      <c r="CG31" s="67"/>
+      <c r="CH31" s="67"/>
+      <c r="CI31" s="67"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B32" s="3"/>
@@ -3931,14 +4089,14 @@
       <c r="BY32" s="3"/>
       <c r="BZ32" s="3"/>
       <c r="CA32" s="3"/>
-      <c r="CB32" s="56"/>
-      <c r="CC32" s="56"/>
-      <c r="CD32" s="56"/>
-      <c r="CE32" s="56"/>
-      <c r="CF32" s="56"/>
-      <c r="CG32" s="56"/>
-      <c r="CH32" s="56"/>
-      <c r="CI32" s="56"/>
+      <c r="CB32" s="67"/>
+      <c r="CC32" s="67"/>
+      <c r="CD32" s="67"/>
+      <c r="CE32" s="67"/>
+      <c r="CF32" s="67"/>
+      <c r="CG32" s="67"/>
+      <c r="CH32" s="67"/>
+      <c r="CI32" s="67"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B33" s="3"/>
@@ -3961,14 +4119,14 @@
       <c r="BY33" s="3"/>
       <c r="BZ33" s="3"/>
       <c r="CA33" s="3"/>
-      <c r="CB33" s="56"/>
-      <c r="CC33" s="56"/>
-      <c r="CD33" s="56"/>
-      <c r="CE33" s="56"/>
-      <c r="CF33" s="56"/>
-      <c r="CG33" s="56"/>
-      <c r="CH33" s="56"/>
-      <c r="CI33" s="56"/>
+      <c r="CB33" s="67"/>
+      <c r="CC33" s="67"/>
+      <c r="CD33" s="67"/>
+      <c r="CE33" s="67"/>
+      <c r="CF33" s="67"/>
+      <c r="CG33" s="67"/>
+      <c r="CH33" s="67"/>
+      <c r="CI33" s="67"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B34" s="3"/>
@@ -4006,14 +4164,14 @@
       <c r="BY34" s="3"/>
       <c r="BZ34" s="3"/>
       <c r="CA34" s="3"/>
-      <c r="CB34" s="56"/>
-      <c r="CC34" s="56"/>
-      <c r="CD34" s="56"/>
-      <c r="CE34" s="56"/>
-      <c r="CF34" s="56"/>
-      <c r="CG34" s="56"/>
-      <c r="CH34" s="56"/>
-      <c r="CI34" s="56"/>
+      <c r="CB34" s="67"/>
+      <c r="CC34" s="67"/>
+      <c r="CD34" s="67"/>
+      <c r="CE34" s="67"/>
+      <c r="CF34" s="67"/>
+      <c r="CG34" s="67"/>
+      <c r="CH34" s="67"/>
+      <c r="CI34" s="67"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B35" s="3"/>
@@ -4051,14 +4209,14 @@
       <c r="BY35" s="3"/>
       <c r="BZ35" s="3"/>
       <c r="CA35" s="3"/>
-      <c r="CB35" s="56"/>
-      <c r="CC35" s="56"/>
-      <c r="CD35" s="56"/>
-      <c r="CE35" s="56"/>
-      <c r="CF35" s="56"/>
-      <c r="CG35" s="56"/>
-      <c r="CH35" s="56"/>
-      <c r="CI35" s="56"/>
+      <c r="CB35" s="67"/>
+      <c r="CC35" s="67"/>
+      <c r="CD35" s="67"/>
+      <c r="CE35" s="67"/>
+      <c r="CF35" s="67"/>
+      <c r="CG35" s="67"/>
+      <c r="CH35" s="67"/>
+      <c r="CI35" s="67"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B36" s="3"/>
@@ -4081,14 +4239,14 @@
       <c r="BY36" s="3"/>
       <c r="BZ36" s="3"/>
       <c r="CA36" s="3"/>
-      <c r="CB36" s="56"/>
-      <c r="CC36" s="56"/>
-      <c r="CD36" s="56"/>
-      <c r="CE36" s="56"/>
-      <c r="CF36" s="56"/>
-      <c r="CG36" s="56"/>
-      <c r="CH36" s="56"/>
-      <c r="CI36" s="56"/>
+      <c r="CB36" s="67"/>
+      <c r="CC36" s="67"/>
+      <c r="CD36" s="67"/>
+      <c r="CE36" s="67"/>
+      <c r="CF36" s="67"/>
+      <c r="CG36" s="67"/>
+      <c r="CH36" s="67"/>
+      <c r="CI36" s="67"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="75:87">
       <c r="BW37" s="3"/>
@@ -4096,14 +4254,14 @@
       <c r="BY37" s="3"/>
       <c r="BZ37" s="3"/>
       <c r="CA37" s="3"/>
-      <c r="CB37" s="56"/>
-      <c r="CC37" s="56"/>
-      <c r="CD37" s="56"/>
-      <c r="CE37" s="56"/>
-      <c r="CF37" s="56"/>
-      <c r="CG37" s="56"/>
-      <c r="CH37" s="56"/>
-      <c r="CI37" s="56"/>
+      <c r="CB37" s="67"/>
+      <c r="CC37" s="67"/>
+      <c r="CD37" s="67"/>
+      <c r="CE37" s="67"/>
+      <c r="CF37" s="67"/>
+      <c r="CG37" s="67"/>
+      <c r="CH37" s="67"/>
+      <c r="CI37" s="67"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="75:87">
       <c r="BW38" s="3"/>
@@ -6596,11 +6754,13 @@
       <c r="CI203" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="200">
+  <mergeCells count="203">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="G3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="AM4:AP4"/>
+    <mergeCell ref="BW4:BX4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:H5"/>
     <mergeCell ref="K5:M5"/>
@@ -6650,7 +6810,7 @@
     <mergeCell ref="AJ18:AM18"/>
     <mergeCell ref="AN18:AP18"/>
     <mergeCell ref="B19:AP19"/>
-    <mergeCell ref="AR19:CI19"/>
+    <mergeCell ref="AR19:CJ19"/>
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="L20:O20"/>
@@ -6663,7 +6823,7 @@
     <mergeCell ref="AN20:AP20"/>
     <mergeCell ref="BW20:BX20"/>
     <mergeCell ref="BY20:BZ20"/>
-    <mergeCell ref="CG20:CI20"/>
+    <mergeCell ref="CH20:CJ20"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="L21:O21"/>
@@ -6676,7 +6836,7 @@
     <mergeCell ref="AN21:AP21"/>
     <mergeCell ref="BW21:BX21"/>
     <mergeCell ref="BY21:BZ21"/>
-    <mergeCell ref="CG21:CI21"/>
+    <mergeCell ref="CH21:CJ21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="G22:K22"/>
     <mergeCell ref="L22:O22"/>
@@ -6689,7 +6849,7 @@
     <mergeCell ref="AN22:AP22"/>
     <mergeCell ref="BW22:BX22"/>
     <mergeCell ref="BY22:BZ22"/>
-    <mergeCell ref="CG22:CI22"/>
+    <mergeCell ref="CH22:CJ22"/>
     <mergeCell ref="C23:F23"/>
     <mergeCell ref="G23:K23"/>
     <mergeCell ref="L23:O23"/>
@@ -6702,7 +6862,7 @@
     <mergeCell ref="AN23:AP23"/>
     <mergeCell ref="BW23:BX23"/>
     <mergeCell ref="BY23:BZ23"/>
-    <mergeCell ref="CG23:CI23"/>
+    <mergeCell ref="CH23:CJ23"/>
     <mergeCell ref="C24:F24"/>
     <mergeCell ref="G24:K24"/>
     <mergeCell ref="L24:O24"/>
@@ -6715,7 +6875,7 @@
     <mergeCell ref="AN24:AP24"/>
     <mergeCell ref="BW24:BX24"/>
     <mergeCell ref="BY24:BZ24"/>
-    <mergeCell ref="CG24:CI24"/>
+    <mergeCell ref="CH24:CJ24"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="G25:K25"/>
     <mergeCell ref="L25:O25"/>
@@ -6728,7 +6888,7 @@
     <mergeCell ref="AN25:AP25"/>
     <mergeCell ref="BW25:BX25"/>
     <mergeCell ref="BY25:BZ25"/>
-    <mergeCell ref="CG25:CI25"/>
+    <mergeCell ref="CH25:CJ25"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="G26:K26"/>
     <mergeCell ref="L26:O26"/>
@@ -6741,7 +6901,7 @@
     <mergeCell ref="AN26:AP26"/>
     <mergeCell ref="BW26:BX26"/>
     <mergeCell ref="BY26:BZ26"/>
-    <mergeCell ref="CG26:CI26"/>
+    <mergeCell ref="CH26:CJ26"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="G27:K27"/>
     <mergeCell ref="L27:O27"/>
@@ -6754,7 +6914,7 @@
     <mergeCell ref="AN27:AP27"/>
     <mergeCell ref="BW27:BX27"/>
     <mergeCell ref="BY27:BZ27"/>
-    <mergeCell ref="CG27:CI27"/>
+    <mergeCell ref="CH27:CJ27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="G28:K28"/>
     <mergeCell ref="L28:O28"/>
@@ -6767,7 +6927,7 @@
     <mergeCell ref="AN28:AP28"/>
     <mergeCell ref="BW28:BX28"/>
     <mergeCell ref="BY28:BZ28"/>
-    <mergeCell ref="CG28:CI28"/>
+    <mergeCell ref="CH28:CJ28"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="G29:K29"/>
     <mergeCell ref="L29:O29"/>
@@ -6780,23 +6940,24 @@
     <mergeCell ref="AN29:AP29"/>
     <mergeCell ref="BW29:BX29"/>
     <mergeCell ref="BY29:BZ29"/>
-    <mergeCell ref="CG29:CI29"/>
+    <mergeCell ref="CH29:CJ29"/>
     <mergeCell ref="CA17:CA18"/>
     <mergeCell ref="CB17:CB18"/>
     <mergeCell ref="CC17:CC18"/>
     <mergeCell ref="CD17:CD18"/>
     <mergeCell ref="CE17:CE18"/>
     <mergeCell ref="CF17:CF18"/>
-    <mergeCell ref="BW3:BX4"/>
-    <mergeCell ref="AJ5:AL9"/>
+    <mergeCell ref="CG17:CG18"/>
     <mergeCell ref="K7:M8"/>
     <mergeCell ref="N7:Q8"/>
     <mergeCell ref="K9:M10"/>
     <mergeCell ref="N9:Q10"/>
-    <mergeCell ref="AJ10:AL15"/>
     <mergeCell ref="BW17:BX18"/>
     <mergeCell ref="BY17:BZ18"/>
-    <mergeCell ref="CG17:CI18"/>
+    <mergeCell ref="BW2:BX3"/>
+    <mergeCell ref="AJ4:AL8"/>
+    <mergeCell ref="AJ9:AL15"/>
+    <mergeCell ref="CH17:CJ18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[#7997] fix excel template
</commit_message>
<xml_diff>
--- a/storage/app/excel/child_application_table.xlsx
+++ b/storage/app/excel/child_application_table.xlsx
@@ -217,10 +217,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -270,6 +270,22 @@
       <charset val="128"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -284,25 +300,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,7 +317,23 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -331,6 +347,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -339,11 +376,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -357,36 +393,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -401,14 +408,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,7 +453,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,37 +507,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -513,13 +525,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -531,61 +597,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,30 +615,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -678,6 +678,26 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -769,6 +789,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -813,13 +844,17 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -834,15 +869,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -866,7 +892,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -889,23 +924,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -925,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -943,134 +963,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1111,26 +1131,26 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="58" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1141,43 +1161,40 @@
     <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="58" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,107 +1203,83 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1609,8 +1602,8 @@
   <sheetPr/>
   <dimension ref="A1:CJ203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1641,41 +1634,41 @@
       <c r="CI1" s="3"/>
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="44:87">
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="37"/>
-      <c r="AX2" s="37"/>
-      <c r="AY2" s="37"/>
-      <c r="AZ2" s="37"/>
-      <c r="BA2" s="37"/>
-      <c r="BB2" s="37"/>
-      <c r="BC2" s="37"/>
-      <c r="BD2" s="37"/>
-      <c r="BE2" s="37"/>
-      <c r="BF2" s="37"/>
-      <c r="BG2" s="37"/>
-      <c r="BH2" s="37"/>
-      <c r="BI2" s="37"/>
-      <c r="BJ2" s="37"/>
-      <c r="BK2" s="37"/>
-      <c r="BL2" s="37"/>
-      <c r="BM2" s="37"/>
-      <c r="BN2" s="37"/>
-      <c r="BO2" s="37"/>
-      <c r="BP2" s="37"/>
-      <c r="BQ2" s="37"/>
-      <c r="BR2" s="37"/>
-      <c r="BS2" s="37"/>
-      <c r="BT2" s="37"/>
-      <c r="BU2" s="37"/>
-      <c r="BV2" s="51"/>
-      <c r="BW2" s="52" t="s">
+      <c r="AR2" s="36"/>
+      <c r="AS2" s="36"/>
+      <c r="AT2" s="36"/>
+      <c r="AU2" s="36"/>
+      <c r="AV2" s="36"/>
+      <c r="AW2" s="36"/>
+      <c r="AX2" s="36"/>
+      <c r="AY2" s="36"/>
+      <c r="AZ2" s="36"/>
+      <c r="BA2" s="36"/>
+      <c r="BB2" s="36"/>
+      <c r="BC2" s="36"/>
+      <c r="BD2" s="36"/>
+      <c r="BE2" s="36"/>
+      <c r="BF2" s="36"/>
+      <c r="BG2" s="36"/>
+      <c r="BH2" s="36"/>
+      <c r="BI2" s="36"/>
+      <c r="BJ2" s="36"/>
+      <c r="BK2" s="36"/>
+      <c r="BL2" s="36"/>
+      <c r="BM2" s="36"/>
+      <c r="BN2" s="36"/>
+      <c r="BO2" s="36"/>
+      <c r="BP2" s="36"/>
+      <c r="BQ2" s="36"/>
+      <c r="BR2" s="36"/>
+      <c r="BS2" s="36"/>
+      <c r="BT2" s="36"/>
+      <c r="BU2" s="36"/>
+      <c r="BV2" s="50"/>
+      <c r="BW2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="BX2" s="37"/>
+      <c r="BX2" s="36"/>
       <c r="BY2" s="3"/>
       <c r="BZ2" s="3"/>
       <c r="CA2" s="3"/>
@@ -1711,39 +1704,39 @@
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="AR3" s="37"/>
-      <c r="AS3" s="37"/>
-      <c r="AT3" s="37"/>
-      <c r="AU3" s="37"/>
-      <c r="AV3" s="37"/>
-      <c r="AW3" s="47"/>
-      <c r="AX3" s="48"/>
-      <c r="AY3" s="37"/>
-      <c r="AZ3" s="37"/>
-      <c r="BA3" s="37"/>
-      <c r="BB3" s="37"/>
-      <c r="BC3" s="37"/>
-      <c r="BD3" s="47"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="37"/>
-      <c r="BG3" s="37"/>
-      <c r="BH3" s="37"/>
-      <c r="BI3" s="37"/>
-      <c r="BJ3" s="37"/>
-      <c r="BK3" s="47"/>
-      <c r="BL3" s="48"/>
-      <c r="BM3" s="37"/>
-      <c r="BN3" s="37"/>
-      <c r="BO3" s="37"/>
-      <c r="BP3" s="37"/>
-      <c r="BQ3" s="37"/>
-      <c r="BR3" s="47"/>
-      <c r="BS3" s="48"/>
-      <c r="BT3" s="37"/>
-      <c r="BU3" s="37"/>
-      <c r="BV3" s="51"/>
-      <c r="BW3" s="52"/>
-      <c r="BX3" s="37"/>
+      <c r="AR3" s="36"/>
+      <c r="AS3" s="36"/>
+      <c r="AT3" s="36"/>
+      <c r="AU3" s="36"/>
+      <c r="AV3" s="36"/>
+      <c r="AW3" s="46"/>
+      <c r="AX3" s="47"/>
+      <c r="AY3" s="36"/>
+      <c r="AZ3" s="36"/>
+      <c r="BA3" s="36"/>
+      <c r="BB3" s="36"/>
+      <c r="BC3" s="36"/>
+      <c r="BD3" s="46"/>
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="36"/>
+      <c r="BG3" s="36"/>
+      <c r="BH3" s="36"/>
+      <c r="BI3" s="36"/>
+      <c r="BJ3" s="36"/>
+      <c r="BK3" s="46"/>
+      <c r="BL3" s="47"/>
+      <c r="BM3" s="36"/>
+      <c r="BN3" s="36"/>
+      <c r="BO3" s="36"/>
+      <c r="BP3" s="36"/>
+      <c r="BQ3" s="36"/>
+      <c r="BR3" s="46"/>
+      <c r="BS3" s="47"/>
+      <c r="BT3" s="36"/>
+      <c r="BU3" s="36"/>
+      <c r="BV3" s="50"/>
+      <c r="BW3" s="51"/>
+      <c r="BX3" s="36"/>
       <c r="BY3" s="3"/>
       <c r="BZ3" s="3"/>
       <c r="CA3" s="3"/>
@@ -1762,13 +1755,13 @@
       </c>
       <c r="AK4" s="8"/>
       <c r="AL4" s="8"/>
-      <c r="AM4" s="27" t="s">
+      <c r="AM4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="38" t="s">
+      <c r="AN4" s="26"/>
+      <c r="AO4" s="26"/>
+      <c r="AP4" s="26"/>
+      <c r="AQ4" s="37" t="s">
         <v>5</v>
       </c>
       <c r="AR4" s="9"/>
@@ -1802,7 +1795,7 @@
       <c r="BT4" s="9"/>
       <c r="BU4" s="9"/>
       <c r="BV4" s="9"/>
-      <c r="BW4" s="53"/>
+      <c r="BW4" s="52"/>
       <c r="BX4" s="9"/>
       <c r="BY4" s="3"/>
       <c r="BZ4" s="3"/>
@@ -1839,13 +1832,13 @@
       <c r="AJ5" s="8"/>
       <c r="AK5" s="8"/>
       <c r="AL5" s="8"/>
-      <c r="AM5" s="27" t="s">
+      <c r="AM5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="AN5" s="27"/>
-      <c r="AO5" s="27"/>
-      <c r="AP5" s="27"/>
-      <c r="AQ5" s="38" t="s">
+      <c r="AN5" s="26"/>
+      <c r="AO5" s="26"/>
+      <c r="AP5" s="26"/>
+      <c r="AQ5" s="37" t="s">
         <v>9</v>
       </c>
       <c r="AR5" s="9"/>
@@ -1879,7 +1872,7 @@
       <c r="BT5" s="9"/>
       <c r="BU5" s="9"/>
       <c r="BV5" s="9"/>
-      <c r="BW5" s="53"/>
+      <c r="BW5" s="52"/>
       <c r="BX5" s="9"/>
       <c r="BY5" s="3"/>
       <c r="BZ5" s="3"/>
@@ -1916,13 +1909,13 @@
       <c r="AJ6" s="8"/>
       <c r="AK6" s="8"/>
       <c r="AL6" s="8"/>
-      <c r="AM6" s="27" t="s">
+      <c r="AM6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="AN6" s="27"/>
-      <c r="AO6" s="27"/>
-      <c r="AP6" s="27"/>
-      <c r="AQ6" s="38" t="s">
+      <c r="AN6" s="26"/>
+      <c r="AO6" s="26"/>
+      <c r="AP6" s="26"/>
+      <c r="AQ6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="AR6" s="9"/>
@@ -1956,7 +1949,7 @@
       <c r="BT6" s="9"/>
       <c r="BU6" s="9"/>
       <c r="BV6" s="9"/>
-      <c r="BW6" s="53"/>
+      <c r="BW6" s="52"/>
       <c r="BX6" s="9"/>
       <c r="BY6" s="3"/>
       <c r="BZ6" s="3"/>
@@ -1993,13 +1986,13 @@
       <c r="AJ7" s="8"/>
       <c r="AK7" s="8"/>
       <c r="AL7" s="8"/>
-      <c r="AM7" s="27" t="s">
+      <c r="AM7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="AN7" s="27"/>
-      <c r="AO7" s="27"/>
-      <c r="AP7" s="27"/>
-      <c r="AQ7" s="38" t="s">
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="26"/>
+      <c r="AQ7" s="37" t="s">
         <v>17</v>
       </c>
       <c r="AR7" s="9"/>
@@ -2033,7 +2026,7 @@
       <c r="BT7" s="9"/>
       <c r="BU7" s="9"/>
       <c r="BV7" s="9"/>
-      <c r="BW7" s="53"/>
+      <c r="BW7" s="52"/>
       <c r="BX7" s="9"/>
       <c r="BY7" s="3"/>
       <c r="BZ7" s="3"/>
@@ -2065,51 +2058,51 @@
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
       <c r="Q8" s="9"/>
-      <c r="AJ8" s="28"/>
-      <c r="AK8" s="28"/>
-      <c r="AL8" s="28"/>
-      <c r="AM8" s="29" t="s">
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AN8" s="29"/>
-      <c r="AO8" s="29"/>
-      <c r="AP8" s="29"/>
-      <c r="AQ8" s="39" t="s">
+      <c r="AN8" s="28"/>
+      <c r="AO8" s="28"/>
+      <c r="AP8" s="28"/>
+      <c r="AQ8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="AR8" s="20"/>
-      <c r="AS8" s="20"/>
-      <c r="AT8" s="20"/>
-      <c r="AU8" s="20"/>
-      <c r="AV8" s="20"/>
-      <c r="AW8" s="20"/>
-      <c r="AX8" s="20"/>
-      <c r="AY8" s="20"/>
-      <c r="AZ8" s="20"/>
-      <c r="BA8" s="20"/>
-      <c r="BB8" s="20"/>
-      <c r="BC8" s="20"/>
-      <c r="BD8" s="20"/>
-      <c r="BE8" s="20"/>
-      <c r="BF8" s="20"/>
-      <c r="BG8" s="20"/>
-      <c r="BH8" s="20"/>
-      <c r="BI8" s="20"/>
-      <c r="BJ8" s="20"/>
-      <c r="BK8" s="20"/>
-      <c r="BL8" s="20"/>
-      <c r="BM8" s="20"/>
-      <c r="BN8" s="20"/>
-      <c r="BO8" s="20"/>
-      <c r="BP8" s="20"/>
-      <c r="BQ8" s="20"/>
-      <c r="BR8" s="20"/>
-      <c r="BS8" s="20"/>
-      <c r="BT8" s="20"/>
-      <c r="BU8" s="20"/>
-      <c r="BV8" s="20"/>
-      <c r="BW8" s="54"/>
-      <c r="BX8" s="20"/>
+      <c r="AR8" s="39"/>
+      <c r="AS8" s="39"/>
+      <c r="AT8" s="39"/>
+      <c r="AU8" s="39"/>
+      <c r="AV8" s="39"/>
+      <c r="AW8" s="39"/>
+      <c r="AX8" s="39"/>
+      <c r="AY8" s="39"/>
+      <c r="AZ8" s="39"/>
+      <c r="BA8" s="39"/>
+      <c r="BB8" s="39"/>
+      <c r="BC8" s="39"/>
+      <c r="BD8" s="39"/>
+      <c r="BE8" s="39"/>
+      <c r="BF8" s="39"/>
+      <c r="BG8" s="39"/>
+      <c r="BH8" s="39"/>
+      <c r="BI8" s="39"/>
+      <c r="BJ8" s="39"/>
+      <c r="BK8" s="39"/>
+      <c r="BL8" s="39"/>
+      <c r="BM8" s="39"/>
+      <c r="BN8" s="39"/>
+      <c r="BO8" s="39"/>
+      <c r="BP8" s="39"/>
+      <c r="BQ8" s="39"/>
+      <c r="BR8" s="39"/>
+      <c r="BS8" s="39"/>
+      <c r="BT8" s="39"/>
+      <c r="BU8" s="39"/>
+      <c r="BV8" s="39"/>
+      <c r="BW8" s="53"/>
+      <c r="BX8" s="39"/>
       <c r="BY8" s="3"/>
       <c r="BZ8" s="3"/>
       <c r="CA8" s="3"/>
@@ -2142,17 +2135,17 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
-      <c r="AJ9" s="30" t="s">
+      <c r="AJ9" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="AK9" s="31"/>
-      <c r="AL9" s="31"/>
-      <c r="AM9" s="32" t="s">
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="30"/>
+      <c r="AM9" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="AN9" s="32"/>
-      <c r="AO9" s="32"/>
-      <c r="AP9" s="32"/>
+      <c r="AN9" s="31"/>
+      <c r="AO9" s="31"/>
+      <c r="AP9" s="31"/>
       <c r="AQ9" s="40" t="s">
         <v>25</v>
       </c>
@@ -2187,7 +2180,7 @@
       <c r="BT9" s="41"/>
       <c r="BU9" s="41"/>
       <c r="BV9" s="41"/>
-      <c r="BW9" s="55"/>
+      <c r="BW9" s="54"/>
       <c r="BX9" s="41"/>
       <c r="BY9" s="3"/>
       <c r="BZ9" s="3"/>
@@ -2219,16 +2212,16 @@
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
-      <c r="AJ10" s="33"/>
-      <c r="AK10" s="34"/>
-      <c r="AL10" s="34"/>
-      <c r="AM10" s="27" t="s">
+      <c r="AJ10" s="32"/>
+      <c r="AK10" s="33"/>
+      <c r="AL10" s="33"/>
+      <c r="AM10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="38" t="s">
+      <c r="AN10" s="26"/>
+      <c r="AO10" s="26"/>
+      <c r="AP10" s="26"/>
+      <c r="AQ10" s="37" t="s">
         <v>28</v>
       </c>
       <c r="AR10" s="9"/>
@@ -2262,7 +2255,7 @@
       <c r="BT10" s="9"/>
       <c r="BU10" s="9"/>
       <c r="BV10" s="9"/>
-      <c r="BW10" s="53"/>
+      <c r="BW10" s="52"/>
       <c r="BX10" s="9"/>
       <c r="BY10" s="3"/>
       <c r="BZ10" s="3"/>
@@ -2292,16 +2285,16 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="AJ11" s="33"/>
-      <c r="AK11" s="34"/>
-      <c r="AL11" s="34"/>
-      <c r="AM11" s="27" t="s">
+      <c r="AJ11" s="32"/>
+      <c r="AK11" s="33"/>
+      <c r="AL11" s="33"/>
+      <c r="AM11" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AN11" s="27"/>
-      <c r="AO11" s="27"/>
-      <c r="AP11" s="27"/>
-      <c r="AQ11" s="38" t="s">
+      <c r="AN11" s="26"/>
+      <c r="AO11" s="26"/>
+      <c r="AP11" s="26"/>
+      <c r="AQ11" s="37" t="s">
         <v>30</v>
       </c>
       <c r="AR11" s="9"/>
@@ -2335,7 +2328,7 @@
       <c r="BT11" s="9"/>
       <c r="BU11" s="9"/>
       <c r="BV11" s="9"/>
-      <c r="BW11" s="53"/>
+      <c r="BW11" s="52"/>
       <c r="BX11" s="9"/>
       <c r="BY11" s="3"/>
       <c r="BZ11" s="3"/>
@@ -2365,16 +2358,16 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="AJ12" s="33"/>
-      <c r="AK12" s="34"/>
-      <c r="AL12" s="34"/>
-      <c r="AM12" s="27" t="s">
+      <c r="AJ12" s="32"/>
+      <c r="AK12" s="33"/>
+      <c r="AL12" s="33"/>
+      <c r="AM12" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AN12" s="27"/>
-      <c r="AO12" s="27"/>
-      <c r="AP12" s="27"/>
-      <c r="AQ12" s="38" t="s">
+      <c r="AN12" s="26"/>
+      <c r="AO12" s="26"/>
+      <c r="AP12" s="26"/>
+      <c r="AQ12" s="37" t="s">
         <v>32</v>
       </c>
       <c r="AR12" s="9"/>
@@ -2408,7 +2401,7 @@
       <c r="BT12" s="9"/>
       <c r="BU12" s="9"/>
       <c r="BV12" s="9"/>
-      <c r="BW12" s="53"/>
+      <c r="BW12" s="52"/>
       <c r="BX12" s="9"/>
       <c r="BY12" s="3"/>
       <c r="BZ12" s="3"/>
@@ -2438,16 +2431,16 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="AJ13" s="33"/>
-      <c r="AK13" s="34"/>
-      <c r="AL13" s="34"/>
-      <c r="AM13" s="27" t="s">
+      <c r="AJ13" s="32"/>
+      <c r="AK13" s="33"/>
+      <c r="AL13" s="33"/>
+      <c r="AM13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="AN13" s="27"/>
-      <c r="AO13" s="27"/>
-      <c r="AP13" s="27"/>
-      <c r="AQ13" s="38" t="s">
+      <c r="AN13" s="26"/>
+      <c r="AO13" s="26"/>
+      <c r="AP13" s="26"/>
+      <c r="AQ13" s="37" t="s">
         <v>34</v>
       </c>
       <c r="AR13" s="9"/>
@@ -2481,7 +2474,7 @@
       <c r="BT13" s="9"/>
       <c r="BU13" s="9"/>
       <c r="BV13" s="9"/>
-      <c r="BW13" s="53"/>
+      <c r="BW13" s="52"/>
       <c r="BX13" s="9"/>
       <c r="BY13" s="3"/>
       <c r="BZ13" s="3"/>
@@ -2511,16 +2504,16 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="AJ14" s="33"/>
-      <c r="AK14" s="34"/>
-      <c r="AL14" s="34"/>
-      <c r="AM14" s="27" t="s">
+      <c r="AJ14" s="32"/>
+      <c r="AK14" s="33"/>
+      <c r="AL14" s="33"/>
+      <c r="AM14" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="AN14" s="27"/>
-      <c r="AO14" s="27"/>
-      <c r="AP14" s="27"/>
-      <c r="AQ14" s="38" t="s">
+      <c r="AN14" s="26"/>
+      <c r="AO14" s="26"/>
+      <c r="AP14" s="26"/>
+      <c r="AQ14" s="37" t="s">
         <v>36</v>
       </c>
       <c r="AR14" s="9"/>
@@ -2554,7 +2547,7 @@
       <c r="BT14" s="9"/>
       <c r="BU14" s="9"/>
       <c r="BV14" s="9"/>
-      <c r="BW14" s="53"/>
+      <c r="BW14" s="52"/>
       <c r="BX14" s="9"/>
       <c r="BY14" s="3"/>
       <c r="BZ14" s="3"/>
@@ -2584,16 +2577,16 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="AJ15" s="35"/>
-      <c r="AK15" s="36"/>
-      <c r="AL15" s="36"/>
-      <c r="AM15" s="27" t="s">
+      <c r="AJ15" s="34"/>
+      <c r="AK15" s="35"/>
+      <c r="AL15" s="35"/>
+      <c r="AM15" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AN15" s="27"/>
-      <c r="AO15" s="27"/>
-      <c r="AP15" s="27"/>
-      <c r="AQ15" s="38" t="s">
+      <c r="AN15" s="26"/>
+      <c r="AO15" s="26"/>
+      <c r="AP15" s="26"/>
+      <c r="AQ15" s="37" t="s">
         <v>38</v>
       </c>
       <c r="AR15" s="9"/>
@@ -2627,7 +2620,7 @@
       <c r="BT15" s="9"/>
       <c r="BU15" s="9"/>
       <c r="BV15" s="9"/>
-      <c r="BW15" s="53"/>
+      <c r="BW15" s="52"/>
       <c r="BX15" s="9"/>
       <c r="BY15" s="3"/>
       <c r="BZ15" s="3"/>
@@ -2672,133 +2665,133 @@
       <c r="CI16" s="3"/>
     </row>
     <row r="17" s="1" customFormat="1" customHeight="1" spans="44:88">
-      <c r="AR17" s="37">
+      <c r="AR17" s="36">
         <v>1</v>
       </c>
-      <c r="AS17" s="37">
+      <c r="AS17" s="36">
         <v>2</v>
       </c>
-      <c r="AT17" s="37">
+      <c r="AT17" s="36">
         <v>3</v>
       </c>
-      <c r="AU17" s="37">
+      <c r="AU17" s="36">
         <v>4</v>
       </c>
-      <c r="AV17" s="37">
+      <c r="AV17" s="36">
         <v>5</v>
       </c>
-      <c r="AW17" s="37">
+      <c r="AW17" s="36">
         <v>6</v>
       </c>
-      <c r="AX17" s="37">
+      <c r="AX17" s="36">
         <v>7</v>
       </c>
-      <c r="AY17" s="37">
+      <c r="AY17" s="36">
         <v>8</v>
       </c>
-      <c r="AZ17" s="37">
+      <c r="AZ17" s="36">
         <v>9</v>
       </c>
-      <c r="BA17" s="37">
+      <c r="BA17" s="36">
         <v>10</v>
       </c>
-      <c r="BB17" s="37">
+      <c r="BB17" s="36">
         <v>11</v>
       </c>
-      <c r="BC17" s="37">
+      <c r="BC17" s="36">
         <v>12</v>
       </c>
-      <c r="BD17" s="37">
+      <c r="BD17" s="36">
         <v>13</v>
       </c>
-      <c r="BE17" s="37">
+      <c r="BE17" s="36">
         <v>14</v>
       </c>
-      <c r="BF17" s="37">
+      <c r="BF17" s="36">
         <v>15</v>
       </c>
-      <c r="BG17" s="37">
+      <c r="BG17" s="36">
         <v>16</v>
       </c>
-      <c r="BH17" s="37">
+      <c r="BH17" s="36">
         <v>17</v>
       </c>
-      <c r="BI17" s="37">
+      <c r="BI17" s="36">
         <v>18</v>
       </c>
-      <c r="BJ17" s="37">
+      <c r="BJ17" s="36">
         <v>19</v>
       </c>
-      <c r="BK17" s="37">
+      <c r="BK17" s="36">
         <v>20</v>
       </c>
-      <c r="BL17" s="37">
+      <c r="BL17" s="36">
         <v>21</v>
       </c>
-      <c r="BM17" s="37">
+      <c r="BM17" s="36">
         <v>22</v>
       </c>
-      <c r="BN17" s="37">
+      <c r="BN17" s="36">
         <v>23</v>
       </c>
-      <c r="BO17" s="37">
+      <c r="BO17" s="36">
         <v>24</v>
       </c>
-      <c r="BP17" s="37">
+      <c r="BP17" s="36">
         <v>25</v>
       </c>
-      <c r="BQ17" s="37">
+      <c r="BQ17" s="36">
         <v>26</v>
       </c>
-      <c r="BR17" s="37">
+      <c r="BR17" s="36">
         <v>27</v>
       </c>
-      <c r="BS17" s="37">
+      <c r="BS17" s="36">
         <v>28</v>
       </c>
-      <c r="BT17" s="37">
+      <c r="BT17" s="36">
         <v>29</v>
       </c>
-      <c r="BU17" s="37">
+      <c r="BU17" s="36">
         <v>30</v>
       </c>
-      <c r="BV17" s="51">
+      <c r="BV17" s="50">
         <v>31</v>
       </c>
-      <c r="BW17" s="56" t="s">
+      <c r="BW17" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="BX17" s="57"/>
-      <c r="BY17" s="58" t="s">
+      <c r="BX17" s="56"/>
+      <c r="BY17" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="BZ17" s="57"/>
-      <c r="CA17" s="59" t="s">
+      <c r="BZ17" s="56"/>
+      <c r="CA17" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="CB17" s="59" t="s">
+      <c r="CB17" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="CC17" s="59" t="s">
+      <c r="CC17" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="CD17" s="59" t="s">
+      <c r="CD17" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="CE17" s="59" t="s">
+      <c r="CE17" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="CF17" s="59" t="s">
+      <c r="CF17" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="CG17" s="59" t="s">
+      <c r="CG17" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="CH17" s="68" t="s">
+      <c r="CH17" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="CI17" s="68"/>
-      <c r="CJ17" s="68"/>
+      <c r="CI17" s="56"/>
+      <c r="CJ17" s="56"/>
     </row>
     <row r="18" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B18" s="10" t="s">
@@ -2880,10 +2873,10 @@
       <c r="AV18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="AW18" s="49" t="s">
+      <c r="AW18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="AX18" s="50" t="s">
+      <c r="AX18" s="49" t="s">
         <v>63</v>
       </c>
       <c r="AY18" s="43" t="s">
@@ -2901,10 +2894,10 @@
       <c r="BC18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BD18" s="49" t="s">
+      <c r="BD18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="BE18" s="50" t="s">
+      <c r="BE18" s="49" t="s">
         <v>63</v>
       </c>
       <c r="BF18" s="43" t="s">
@@ -2922,10 +2915,10 @@
       <c r="BJ18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BK18" s="49" t="s">
+      <c r="BK18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="BL18" s="50" t="s">
+      <c r="BL18" s="49" t="s">
         <v>63</v>
       </c>
       <c r="BM18" s="43" t="s">
@@ -2943,10 +2936,10 @@
       <c r="BQ18" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BR18" s="49" t="s">
+      <c r="BR18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="BS18" s="50" t="s">
+      <c r="BS18" s="49" t="s">
         <v>63</v>
       </c>
       <c r="BT18" s="43" t="s">
@@ -2955,23 +2948,23 @@
       <c r="BU18" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="BV18" s="60" t="s">
+      <c r="BV18" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="BW18" s="61"/>
-      <c r="BX18" s="62"/>
-      <c r="BY18" s="62"/>
-      <c r="BZ18" s="62"/>
-      <c r="CA18" s="63"/>
-      <c r="CB18" s="63"/>
-      <c r="CC18" s="63"/>
-      <c r="CD18" s="63"/>
-      <c r="CE18" s="63"/>
-      <c r="CF18" s="63"/>
-      <c r="CG18" s="63"/>
-      <c r="CH18" s="68"/>
-      <c r="CI18" s="68"/>
-      <c r="CJ18" s="68"/>
+      <c r="BW18" s="60"/>
+      <c r="BX18" s="61"/>
+      <c r="BY18" s="61"/>
+      <c r="BZ18" s="61"/>
+      <c r="CA18" s="62"/>
+      <c r="CB18" s="62"/>
+      <c r="CC18" s="62"/>
+      <c r="CD18" s="62"/>
+      <c r="CE18" s="62"/>
+      <c r="CF18" s="62"/>
+      <c r="CG18" s="62"/>
+      <c r="CH18" s="56"/>
+      <c r="CI18" s="56"/>
+      <c r="CJ18" s="56"/>
     </row>
     <row r="19" s="1" customFormat="1" customHeight="1" spans="2:88">
       <c r="B19" s="14"/>
@@ -3062,730 +3055,729 @@
       <c r="CI19" s="45"/>
       <c r="CJ19" s="45"/>
     </row>
-    <row r="20" s="2" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B20" s="16">
-        <v>1</v>
-      </c>
-      <c r="C20" s="17"/>
+    <row r="20" s="2" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
-      <c r="T20" s="18"/>
-      <c r="U20" s="18"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="18"/>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="18"/>
-      <c r="AB20" s="18"/>
-      <c r="AC20" s="18"/>
-      <c r="AD20" s="18"/>
-      <c r="AE20" s="18"/>
-      <c r="AF20" s="18"/>
-      <c r="AG20" s="18"/>
-      <c r="AH20" s="18"/>
-      <c r="AI20" s="18"/>
-      <c r="AJ20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="17"/>
+      <c r="AI20" s="17"/>
+      <c r="AJ20" s="18"/>
       <c r="AK20" s="18"/>
       <c r="AL20" s="18"/>
       <c r="AM20" s="18"/>
-      <c r="AN20" s="18"/>
-      <c r="AO20" s="18"/>
-      <c r="AP20" s="18"/>
-      <c r="AR20" s="18"/>
-      <c r="AS20" s="18"/>
-      <c r="AT20" s="18"/>
-      <c r="AU20" s="18"/>
-      <c r="AV20" s="18"/>
-      <c r="AW20" s="18"/>
-      <c r="AX20" s="18"/>
-      <c r="AY20" s="18"/>
-      <c r="AZ20" s="18"/>
-      <c r="BA20" s="18"/>
-      <c r="BB20" s="18"/>
-      <c r="BC20" s="18"/>
-      <c r="BD20" s="18"/>
-      <c r="BE20" s="18"/>
-      <c r="BF20" s="18"/>
-      <c r="BG20" s="18"/>
-      <c r="BH20" s="18"/>
-      <c r="BI20" s="18"/>
-      <c r="BJ20" s="18"/>
-      <c r="BK20" s="18"/>
-      <c r="BL20" s="18"/>
-      <c r="BM20" s="18"/>
-      <c r="BN20" s="18"/>
-      <c r="BO20" s="18"/>
-      <c r="BP20" s="18"/>
-      <c r="BQ20" s="18"/>
-      <c r="BR20" s="18"/>
-      <c r="BS20" s="18"/>
-      <c r="BT20" s="18"/>
-      <c r="BU20" s="18"/>
-      <c r="BV20" s="64"/>
-      <c r="BW20" s="65"/>
-      <c r="BX20" s="18"/>
-      <c r="BY20" s="18"/>
-      <c r="BZ20" s="18"/>
-      <c r="CA20" s="18"/>
-      <c r="CB20" s="18"/>
-      <c r="CC20" s="18"/>
-      <c r="CD20" s="18"/>
-      <c r="CE20" s="18"/>
-      <c r="CF20" s="18"/>
-      <c r="CG20" s="16"/>
-      <c r="CH20" s="69"/>
-      <c r="CI20" s="70"/>
-      <c r="CJ20" s="71"/>
-    </row>
-    <row r="21" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B21" s="19">
-        <v>2</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
+      <c r="AN20" s="17"/>
+      <c r="AO20" s="17"/>
+      <c r="AP20" s="17"/>
+      <c r="AQ20" s="16"/>
+      <c r="AR20" s="17"/>
+      <c r="AS20" s="17"/>
+      <c r="AT20" s="17"/>
+      <c r="AU20" s="17"/>
+      <c r="AV20" s="17"/>
+      <c r="AW20" s="17"/>
+      <c r="AX20" s="17"/>
+      <c r="AY20" s="17"/>
+      <c r="AZ20" s="17"/>
+      <c r="BA20" s="17"/>
+      <c r="BB20" s="17"/>
+      <c r="BC20" s="17"/>
+      <c r="BD20" s="17"/>
+      <c r="BE20" s="17"/>
+      <c r="BF20" s="17"/>
+      <c r="BG20" s="17"/>
+      <c r="BH20" s="17"/>
+      <c r="BI20" s="17"/>
+      <c r="BJ20" s="17"/>
+      <c r="BK20" s="17"/>
+      <c r="BL20" s="17"/>
+      <c r="BM20" s="17"/>
+      <c r="BN20" s="17"/>
+      <c r="BO20" s="17"/>
+      <c r="BP20" s="17"/>
+      <c r="BQ20" s="17"/>
+      <c r="BR20" s="17"/>
+      <c r="BS20" s="17"/>
+      <c r="BT20" s="17"/>
+      <c r="BU20" s="17"/>
+      <c r="BV20" s="17"/>
+      <c r="BW20" s="17"/>
+      <c r="BX20" s="17"/>
+      <c r="BY20" s="17"/>
+      <c r="BZ20" s="17"/>
+      <c r="CA20" s="17"/>
+      <c r="CB20" s="17"/>
+      <c r="CC20" s="17"/>
+      <c r="CD20" s="17"/>
+      <c r="CE20" s="17"/>
+      <c r="CF20" s="17"/>
+      <c r="CG20" s="17"/>
+      <c r="CH20" s="17"/>
+      <c r="CI20" s="17"/>
+      <c r="CJ20" s="17"/>
+    </row>
+    <row r="21" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="9"/>
-      <c r="Y21" s="9"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-      <c r="AB21" s="9"/>
-      <c r="AC21" s="9"/>
-      <c r="AD21" s="9"/>
-      <c r="AE21" s="9"/>
-      <c r="AF21" s="9"/>
-      <c r="AG21" s="9"/>
-      <c r="AH21" s="9"/>
-      <c r="AI21" s="9"/>
-      <c r="AJ21" s="9"/>
-      <c r="AK21" s="9"/>
-      <c r="AL21" s="9"/>
-      <c r="AM21" s="9"/>
-      <c r="AN21" s="9"/>
-      <c r="AO21" s="9"/>
-      <c r="AP21" s="9"/>
-      <c r="AR21" s="9"/>
-      <c r="AS21" s="9"/>
-      <c r="AT21" s="9"/>
-      <c r="AU21" s="9"/>
-      <c r="AV21" s="9"/>
-      <c r="AW21" s="9"/>
-      <c r="AX21" s="9"/>
-      <c r="AY21" s="9"/>
-      <c r="AZ21" s="9"/>
-      <c r="BA21" s="9"/>
-      <c r="BB21" s="9"/>
-      <c r="BC21" s="9"/>
-      <c r="BD21" s="9"/>
-      <c r="BE21" s="9"/>
-      <c r="BF21" s="9"/>
-      <c r="BG21" s="9"/>
-      <c r="BH21" s="9"/>
-      <c r="BI21" s="9"/>
-      <c r="BJ21" s="9"/>
-      <c r="BK21" s="9"/>
-      <c r="BL21" s="9"/>
-      <c r="BM21" s="9"/>
-      <c r="BN21" s="9"/>
-      <c r="BO21" s="9"/>
-      <c r="BP21" s="9"/>
-      <c r="BQ21" s="9"/>
-      <c r="BR21" s="9"/>
-      <c r="BS21" s="9"/>
-      <c r="BT21" s="9"/>
-      <c r="BU21" s="9"/>
-      <c r="BV21" s="6"/>
-      <c r="BW21" s="53"/>
-      <c r="BX21" s="9"/>
-      <c r="BY21" s="9"/>
-      <c r="BZ21" s="9"/>
-      <c r="CA21" s="9"/>
-      <c r="CB21" s="9"/>
-      <c r="CC21" s="9"/>
-      <c r="CD21" s="9"/>
-      <c r="CE21" s="9"/>
-      <c r="CF21" s="9"/>
-      <c r="CG21" s="19"/>
-      <c r="CH21" s="69"/>
-      <c r="CI21" s="70"/>
-      <c r="CJ21" s="71"/>
-    </row>
-    <row r="22" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B22" s="19">
-        <v>3</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="20"/>
+      <c r="AB21" s="20"/>
+      <c r="AC21" s="20"/>
+      <c r="AD21" s="20"/>
+      <c r="AE21" s="20"/>
+      <c r="AF21" s="20"/>
+      <c r="AG21" s="20"/>
+      <c r="AH21" s="20"/>
+      <c r="AI21" s="20"/>
+      <c r="AJ21" s="20"/>
+      <c r="AK21" s="20"/>
+      <c r="AL21" s="20"/>
+      <c r="AM21" s="20"/>
+      <c r="AN21" s="20"/>
+      <c r="AO21" s="20"/>
+      <c r="AP21" s="20"/>
+      <c r="AQ21" s="19"/>
+      <c r="AR21" s="20"/>
+      <c r="AS21" s="20"/>
+      <c r="AT21" s="20"/>
+      <c r="AU21" s="20"/>
+      <c r="AV21" s="20"/>
+      <c r="AW21" s="20"/>
+      <c r="AX21" s="20"/>
+      <c r="AY21" s="20"/>
+      <c r="AZ21" s="20"/>
+      <c r="BA21" s="20"/>
+      <c r="BB21" s="20"/>
+      <c r="BC21" s="20"/>
+      <c r="BD21" s="20"/>
+      <c r="BE21" s="20"/>
+      <c r="BF21" s="20"/>
+      <c r="BG21" s="20"/>
+      <c r="BH21" s="20"/>
+      <c r="BI21" s="20"/>
+      <c r="BJ21" s="20"/>
+      <c r="BK21" s="20"/>
+      <c r="BL21" s="20"/>
+      <c r="BM21" s="20"/>
+      <c r="BN21" s="20"/>
+      <c r="BO21" s="20"/>
+      <c r="BP21" s="20"/>
+      <c r="BQ21" s="20"/>
+      <c r="BR21" s="20"/>
+      <c r="BS21" s="20"/>
+      <c r="BT21" s="20"/>
+      <c r="BU21" s="20"/>
+      <c r="BV21" s="20"/>
+      <c r="BW21" s="20"/>
+      <c r="BX21" s="20"/>
+      <c r="BY21" s="20"/>
+      <c r="BZ21" s="20"/>
+      <c r="CA21" s="20"/>
+      <c r="CB21" s="20"/>
+      <c r="CC21" s="20"/>
+      <c r="CD21" s="20"/>
+      <c r="CE21" s="20"/>
+      <c r="CF21" s="20"/>
+      <c r="CG21" s="20"/>
+      <c r="CH21" s="17"/>
+      <c r="CI21" s="17"/>
+      <c r="CJ21" s="17"/>
+    </row>
+    <row r="22" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
       <c r="N22" s="25"/>
       <c r="O22" s="25"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="9"/>
-      <c r="X22" s="9"/>
-      <c r="Y22" s="9"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-      <c r="AB22" s="9"/>
-      <c r="AC22" s="9"/>
-      <c r="AD22" s="9"/>
-      <c r="AE22" s="9"/>
-      <c r="AF22" s="9"/>
-      <c r="AG22" s="9"/>
-      <c r="AH22" s="9"/>
-      <c r="AI22" s="9"/>
-      <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
-      <c r="AL22" s="9"/>
-      <c r="AM22" s="9"/>
-      <c r="AN22" s="9"/>
-      <c r="AO22" s="9"/>
-      <c r="AP22" s="9"/>
-      <c r="AR22" s="9"/>
-      <c r="AS22" s="9"/>
-      <c r="AT22" s="9"/>
-      <c r="AU22" s="9"/>
-      <c r="AV22" s="9"/>
-      <c r="AW22" s="9"/>
-      <c r="AX22" s="9"/>
-      <c r="AY22" s="9"/>
-      <c r="AZ22" s="9"/>
-      <c r="BA22" s="9"/>
-      <c r="BB22" s="9"/>
-      <c r="BC22" s="9"/>
-      <c r="BD22" s="9"/>
-      <c r="BE22" s="9"/>
-      <c r="BF22" s="9"/>
-      <c r="BG22" s="9"/>
-      <c r="BH22" s="9"/>
-      <c r="BI22" s="9"/>
-      <c r="BJ22" s="9"/>
-      <c r="BK22" s="9"/>
-      <c r="BL22" s="9"/>
-      <c r="BM22" s="9"/>
-      <c r="BN22" s="9"/>
-      <c r="BO22" s="9"/>
-      <c r="BP22" s="9"/>
-      <c r="BQ22" s="9"/>
-      <c r="BR22" s="9"/>
-      <c r="BS22" s="9"/>
-      <c r="BT22" s="9"/>
-      <c r="BU22" s="9"/>
-      <c r="BV22" s="6"/>
-      <c r="BW22" s="53"/>
-      <c r="BX22" s="9"/>
-      <c r="BY22" s="9"/>
-      <c r="BZ22" s="9"/>
-      <c r="CA22" s="9"/>
-      <c r="CB22" s="9"/>
-      <c r="CC22" s="9"/>
-      <c r="CD22" s="9"/>
-      <c r="CE22" s="9"/>
-      <c r="CF22" s="9"/>
-      <c r="CG22" s="19"/>
-      <c r="CH22" s="69"/>
-      <c r="CI22" s="70"/>
-      <c r="CJ22" s="71"/>
-    </row>
-    <row r="23" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B23" s="19">
-        <v>4</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="20"/>
+      <c r="AC22" s="20"/>
+      <c r="AD22" s="20"/>
+      <c r="AE22" s="20"/>
+      <c r="AF22" s="20"/>
+      <c r="AG22" s="20"/>
+      <c r="AH22" s="20"/>
+      <c r="AI22" s="20"/>
+      <c r="AJ22" s="20"/>
+      <c r="AK22" s="20"/>
+      <c r="AL22" s="20"/>
+      <c r="AM22" s="20"/>
+      <c r="AN22" s="20"/>
+      <c r="AO22" s="20"/>
+      <c r="AP22" s="20"/>
+      <c r="AQ22" s="19"/>
+      <c r="AR22" s="20"/>
+      <c r="AS22" s="20"/>
+      <c r="AT22" s="20"/>
+      <c r="AU22" s="20"/>
+      <c r="AV22" s="20"/>
+      <c r="AW22" s="20"/>
+      <c r="AX22" s="20"/>
+      <c r="AY22" s="20"/>
+      <c r="AZ22" s="20"/>
+      <c r="BA22" s="20"/>
+      <c r="BB22" s="20"/>
+      <c r="BC22" s="20"/>
+      <c r="BD22" s="20"/>
+      <c r="BE22" s="20"/>
+      <c r="BF22" s="20"/>
+      <c r="BG22" s="20"/>
+      <c r="BH22" s="20"/>
+      <c r="BI22" s="20"/>
+      <c r="BJ22" s="20"/>
+      <c r="BK22" s="20"/>
+      <c r="BL22" s="20"/>
+      <c r="BM22" s="20"/>
+      <c r="BN22" s="20"/>
+      <c r="BO22" s="20"/>
+      <c r="BP22" s="20"/>
+      <c r="BQ22" s="20"/>
+      <c r="BR22" s="20"/>
+      <c r="BS22" s="20"/>
+      <c r="BT22" s="20"/>
+      <c r="BU22" s="20"/>
+      <c r="BV22" s="20"/>
+      <c r="BW22" s="20"/>
+      <c r="BX22" s="20"/>
+      <c r="BY22" s="20"/>
+      <c r="BZ22" s="20"/>
+      <c r="CA22" s="20"/>
+      <c r="CB22" s="20"/>
+      <c r="CC22" s="20"/>
+      <c r="CD22" s="20"/>
+      <c r="CE22" s="20"/>
+      <c r="CF22" s="20"/>
+      <c r="CG22" s="20"/>
+      <c r="CH22" s="17"/>
+      <c r="CI22" s="17"/>
+      <c r="CJ22" s="17"/>
+    </row>
+    <row r="23" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
       <c r="N23" s="25"/>
       <c r="O23" s="25"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
-      <c r="W23" s="9"/>
-      <c r="X23" s="9"/>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
-      <c r="AB23" s="9"/>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-      <c r="AE23" s="9"/>
-      <c r="AF23" s="9"/>
-      <c r="AG23" s="9"/>
-      <c r="AH23" s="9"/>
-      <c r="AI23" s="9"/>
-      <c r="AJ23" s="9"/>
-      <c r="AK23" s="9"/>
-      <c r="AL23" s="9"/>
-      <c r="AM23" s="9"/>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
-      <c r="AP23" s="9"/>
-      <c r="AR23" s="9"/>
-      <c r="AS23" s="9"/>
-      <c r="AT23" s="9"/>
-      <c r="AU23" s="9"/>
-      <c r="AV23" s="9"/>
-      <c r="AW23" s="9"/>
-      <c r="AX23" s="9"/>
-      <c r="AY23" s="9"/>
-      <c r="AZ23" s="9"/>
-      <c r="BA23" s="9"/>
-      <c r="BB23" s="9"/>
-      <c r="BC23" s="9"/>
-      <c r="BD23" s="9"/>
-      <c r="BE23" s="9"/>
-      <c r="BF23" s="9"/>
-      <c r="BG23" s="9"/>
-      <c r="BH23" s="9"/>
-      <c r="BI23" s="9"/>
-      <c r="BJ23" s="9"/>
-      <c r="BK23" s="9"/>
-      <c r="BL23" s="9"/>
-      <c r="BM23" s="9"/>
-      <c r="BN23" s="9"/>
-      <c r="BO23" s="9"/>
-      <c r="BP23" s="9"/>
-      <c r="BQ23" s="9"/>
-      <c r="BR23" s="9"/>
-      <c r="BS23" s="9"/>
-      <c r="BT23" s="9"/>
-      <c r="BU23" s="9"/>
-      <c r="BV23" s="6"/>
-      <c r="BW23" s="53"/>
-      <c r="BX23" s="9"/>
-      <c r="BY23" s="9"/>
-      <c r="BZ23" s="9"/>
-      <c r="CA23" s="9"/>
-      <c r="CB23" s="9"/>
-      <c r="CC23" s="9"/>
-      <c r="CD23" s="9"/>
-      <c r="CE23" s="9"/>
-      <c r="CF23" s="9"/>
-      <c r="CG23" s="19"/>
-      <c r="CH23" s="69"/>
-      <c r="CI23" s="70"/>
-      <c r="CJ23" s="71"/>
-    </row>
-    <row r="24" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B24" s="19">
-        <v>5</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="20"/>
+      <c r="Z23" s="20"/>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="20"/>
+      <c r="AD23" s="20"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="20"/>
+      <c r="AH23" s="20"/>
+      <c r="AI23" s="20"/>
+      <c r="AJ23" s="20"/>
+      <c r="AK23" s="20"/>
+      <c r="AL23" s="20"/>
+      <c r="AM23" s="20"/>
+      <c r="AN23" s="20"/>
+      <c r="AO23" s="20"/>
+      <c r="AP23" s="20"/>
+      <c r="AQ23" s="19"/>
+      <c r="AR23" s="20"/>
+      <c r="AS23" s="20"/>
+      <c r="AT23" s="20"/>
+      <c r="AU23" s="20"/>
+      <c r="AV23" s="20"/>
+      <c r="AW23" s="20"/>
+      <c r="AX23" s="20"/>
+      <c r="AY23" s="20"/>
+      <c r="AZ23" s="20"/>
+      <c r="BA23" s="20"/>
+      <c r="BB23" s="20"/>
+      <c r="BC23" s="20"/>
+      <c r="BD23" s="20"/>
+      <c r="BE23" s="20"/>
+      <c r="BF23" s="20"/>
+      <c r="BG23" s="20"/>
+      <c r="BH23" s="20"/>
+      <c r="BI23" s="20"/>
+      <c r="BJ23" s="20"/>
+      <c r="BK23" s="20"/>
+      <c r="BL23" s="20"/>
+      <c r="BM23" s="20"/>
+      <c r="BN23" s="20"/>
+      <c r="BO23" s="20"/>
+      <c r="BP23" s="20"/>
+      <c r="BQ23" s="20"/>
+      <c r="BR23" s="20"/>
+      <c r="BS23" s="20"/>
+      <c r="BT23" s="20"/>
+      <c r="BU23" s="20"/>
+      <c r="BV23" s="20"/>
+      <c r="BW23" s="20"/>
+      <c r="BX23" s="20"/>
+      <c r="BY23" s="20"/>
+      <c r="BZ23" s="20"/>
+      <c r="CA23" s="20"/>
+      <c r="CB23" s="20"/>
+      <c r="CC23" s="20"/>
+      <c r="CD23" s="20"/>
+      <c r="CE23" s="20"/>
+      <c r="CF23" s="20"/>
+      <c r="CG23" s="20"/>
+      <c r="CH23" s="17"/>
+      <c r="CI23" s="17"/>
+      <c r="CJ23" s="17"/>
+    </row>
+    <row r="24" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
       <c r="N24" s="25"/>
       <c r="O24" s="25"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
-      <c r="W24" s="9"/>
-      <c r="X24" s="9"/>
-      <c r="Y24" s="9"/>
-      <c r="Z24" s="9"/>
-      <c r="AA24" s="9"/>
-      <c r="AB24" s="9"/>
-      <c r="AC24" s="9"/>
-      <c r="AD24" s="9"/>
-      <c r="AE24" s="9"/>
-      <c r="AF24" s="9"/>
-      <c r="AG24" s="9"/>
-      <c r="AH24" s="9"/>
-      <c r="AI24" s="9"/>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="9"/>
-      <c r="AL24" s="9"/>
-      <c r="AM24" s="9"/>
-      <c r="AN24" s="9"/>
-      <c r="AO24" s="9"/>
-      <c r="AP24" s="9"/>
-      <c r="AR24" s="9"/>
-      <c r="AS24" s="9"/>
-      <c r="AT24" s="9"/>
-      <c r="AU24" s="9"/>
-      <c r="AV24" s="9"/>
-      <c r="AW24" s="9"/>
-      <c r="AX24" s="9"/>
-      <c r="AY24" s="9"/>
-      <c r="AZ24" s="9"/>
-      <c r="BA24" s="9"/>
-      <c r="BB24" s="9"/>
-      <c r="BC24" s="9"/>
-      <c r="BD24" s="9"/>
-      <c r="BE24" s="9"/>
-      <c r="BF24" s="9"/>
-      <c r="BG24" s="9"/>
-      <c r="BH24" s="9"/>
-      <c r="BI24" s="9"/>
-      <c r="BJ24" s="9"/>
-      <c r="BK24" s="9"/>
-      <c r="BL24" s="9"/>
-      <c r="BM24" s="9"/>
-      <c r="BN24" s="9"/>
-      <c r="BO24" s="9"/>
-      <c r="BP24" s="9"/>
-      <c r="BQ24" s="9"/>
-      <c r="BR24" s="9"/>
-      <c r="BS24" s="9"/>
-      <c r="BT24" s="9"/>
-      <c r="BU24" s="9"/>
-      <c r="BV24" s="6"/>
-      <c r="BW24" s="53"/>
-      <c r="BX24" s="9"/>
-      <c r="BY24" s="9"/>
-      <c r="BZ24" s="9"/>
-      <c r="CA24" s="9"/>
-      <c r="CB24" s="9"/>
-      <c r="CC24" s="9"/>
-      <c r="CD24" s="9"/>
-      <c r="CE24" s="9"/>
-      <c r="CF24" s="9"/>
-      <c r="CG24" s="19"/>
-      <c r="CH24" s="69"/>
-      <c r="CI24" s="70"/>
-      <c r="CJ24" s="71"/>
-    </row>
-    <row r="25" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B25" s="19">
-        <v>6</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="20"/>
+      <c r="T24" s="20"/>
+      <c r="U24" s="20"/>
+      <c r="V24" s="20"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="20"/>
+      <c r="Y24" s="20"/>
+      <c r="Z24" s="20"/>
+      <c r="AA24" s="20"/>
+      <c r="AB24" s="20"/>
+      <c r="AC24" s="20"/>
+      <c r="AD24" s="20"/>
+      <c r="AE24" s="20"/>
+      <c r="AF24" s="20"/>
+      <c r="AG24" s="20"/>
+      <c r="AH24" s="20"/>
+      <c r="AI24" s="20"/>
+      <c r="AJ24" s="20"/>
+      <c r="AK24" s="20"/>
+      <c r="AL24" s="20"/>
+      <c r="AM24" s="20"/>
+      <c r="AN24" s="20"/>
+      <c r="AO24" s="20"/>
+      <c r="AP24" s="20"/>
+      <c r="AQ24" s="19"/>
+      <c r="AR24" s="20"/>
+      <c r="AS24" s="20"/>
+      <c r="AT24" s="20"/>
+      <c r="AU24" s="20"/>
+      <c r="AV24" s="20"/>
+      <c r="AW24" s="20"/>
+      <c r="AX24" s="20"/>
+      <c r="AY24" s="20"/>
+      <c r="AZ24" s="20"/>
+      <c r="BA24" s="20"/>
+      <c r="BB24" s="20"/>
+      <c r="BC24" s="20"/>
+      <c r="BD24" s="20"/>
+      <c r="BE24" s="20"/>
+      <c r="BF24" s="20"/>
+      <c r="BG24" s="20"/>
+      <c r="BH24" s="20"/>
+      <c r="BI24" s="20"/>
+      <c r="BJ24" s="20"/>
+      <c r="BK24" s="20"/>
+      <c r="BL24" s="20"/>
+      <c r="BM24" s="20"/>
+      <c r="BN24" s="20"/>
+      <c r="BO24" s="20"/>
+      <c r="BP24" s="20"/>
+      <c r="BQ24" s="20"/>
+      <c r="BR24" s="20"/>
+      <c r="BS24" s="20"/>
+      <c r="BT24" s="20"/>
+      <c r="BU24" s="20"/>
+      <c r="BV24" s="20"/>
+      <c r="BW24" s="20"/>
+      <c r="BX24" s="20"/>
+      <c r="BY24" s="20"/>
+      <c r="BZ24" s="20"/>
+      <c r="CA24" s="20"/>
+      <c r="CB24" s="20"/>
+      <c r="CC24" s="20"/>
+      <c r="CD24" s="20"/>
+      <c r="CE24" s="20"/>
+      <c r="CF24" s="20"/>
+      <c r="CG24" s="20"/>
+      <c r="CH24" s="17"/>
+      <c r="CI24" s="17"/>
+      <c r="CJ24" s="17"/>
+    </row>
+    <row r="25" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
-      <c r="W25" s="9"/>
-      <c r="X25" s="9"/>
-      <c r="Y25" s="9"/>
-      <c r="Z25" s="9"/>
-      <c r="AA25" s="9"/>
-      <c r="AB25" s="9"/>
-      <c r="AC25" s="9"/>
-      <c r="AD25" s="9"/>
-      <c r="AE25" s="9"/>
-      <c r="AF25" s="9"/>
-      <c r="AG25" s="9"/>
-      <c r="AH25" s="9"/>
-      <c r="AI25" s="9"/>
-      <c r="AJ25" s="9"/>
-      <c r="AK25" s="9"/>
-      <c r="AL25" s="9"/>
-      <c r="AM25" s="9"/>
-      <c r="AN25" s="9"/>
-      <c r="AO25" s="9"/>
-      <c r="AP25" s="9"/>
-      <c r="AR25" s="9"/>
-      <c r="AS25" s="9"/>
-      <c r="AT25" s="9"/>
-      <c r="AU25" s="9"/>
-      <c r="AV25" s="9"/>
-      <c r="AW25" s="9"/>
-      <c r="AX25" s="9"/>
-      <c r="AY25" s="9"/>
-      <c r="AZ25" s="9"/>
-      <c r="BA25" s="9"/>
-      <c r="BB25" s="9"/>
-      <c r="BC25" s="9"/>
-      <c r="BD25" s="9"/>
-      <c r="BE25" s="9"/>
-      <c r="BF25" s="9"/>
-      <c r="BG25" s="9"/>
-      <c r="BH25" s="9"/>
-      <c r="BI25" s="9"/>
-      <c r="BJ25" s="9"/>
-      <c r="BK25" s="9"/>
-      <c r="BL25" s="9"/>
-      <c r="BM25" s="9"/>
-      <c r="BN25" s="9"/>
-      <c r="BO25" s="9"/>
-      <c r="BP25" s="9"/>
-      <c r="BQ25" s="9"/>
-      <c r="BR25" s="9"/>
-      <c r="BS25" s="9"/>
-      <c r="BT25" s="9"/>
-      <c r="BU25" s="9"/>
-      <c r="BV25" s="6"/>
-      <c r="BW25" s="53"/>
-      <c r="BX25" s="9"/>
-      <c r="BY25" s="9"/>
-      <c r="BZ25" s="9"/>
-      <c r="CA25" s="9"/>
-      <c r="CB25" s="9"/>
-      <c r="CC25" s="9"/>
-      <c r="CD25" s="9"/>
-      <c r="CE25" s="9"/>
-      <c r="CF25" s="9"/>
-      <c r="CG25" s="19"/>
-      <c r="CH25" s="69"/>
-      <c r="CI25" s="70"/>
-      <c r="CJ25" s="71"/>
-    </row>
-    <row r="26" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B26" s="19">
-        <v>7</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="20"/>
+      <c r="U25" s="20"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="20"/>
+      <c r="X25" s="20"/>
+      <c r="Y25" s="20"/>
+      <c r="Z25" s="20"/>
+      <c r="AA25" s="20"/>
+      <c r="AB25" s="20"/>
+      <c r="AC25" s="20"/>
+      <c r="AD25" s="20"/>
+      <c r="AE25" s="20"/>
+      <c r="AF25" s="20"/>
+      <c r="AG25" s="20"/>
+      <c r="AH25" s="20"/>
+      <c r="AI25" s="20"/>
+      <c r="AJ25" s="20"/>
+      <c r="AK25" s="20"/>
+      <c r="AL25" s="20"/>
+      <c r="AM25" s="20"/>
+      <c r="AN25" s="20"/>
+      <c r="AO25" s="20"/>
+      <c r="AP25" s="20"/>
+      <c r="AQ25" s="19"/>
+      <c r="AR25" s="20"/>
+      <c r="AS25" s="20"/>
+      <c r="AT25" s="20"/>
+      <c r="AU25" s="20"/>
+      <c r="AV25" s="20"/>
+      <c r="AW25" s="20"/>
+      <c r="AX25" s="20"/>
+      <c r="AY25" s="20"/>
+      <c r="AZ25" s="20"/>
+      <c r="BA25" s="20"/>
+      <c r="BB25" s="20"/>
+      <c r="BC25" s="20"/>
+      <c r="BD25" s="20"/>
+      <c r="BE25" s="20"/>
+      <c r="BF25" s="20"/>
+      <c r="BG25" s="20"/>
+      <c r="BH25" s="20"/>
+      <c r="BI25" s="20"/>
+      <c r="BJ25" s="20"/>
+      <c r="BK25" s="20"/>
+      <c r="BL25" s="20"/>
+      <c r="BM25" s="20"/>
+      <c r="BN25" s="20"/>
+      <c r="BO25" s="20"/>
+      <c r="BP25" s="20"/>
+      <c r="BQ25" s="20"/>
+      <c r="BR25" s="20"/>
+      <c r="BS25" s="20"/>
+      <c r="BT25" s="20"/>
+      <c r="BU25" s="20"/>
+      <c r="BV25" s="20"/>
+      <c r="BW25" s="20"/>
+      <c r="BX25" s="20"/>
+      <c r="BY25" s="20"/>
+      <c r="BZ25" s="20"/>
+      <c r="CA25" s="20"/>
+      <c r="CB25" s="20"/>
+      <c r="CC25" s="20"/>
+      <c r="CD25" s="20"/>
+      <c r="CE25" s="20"/>
+      <c r="CF25" s="20"/>
+      <c r="CG25" s="20"/>
+      <c r="CH25" s="17"/>
+      <c r="CI25" s="17"/>
+      <c r="CJ25" s="17"/>
+    </row>
+    <row r="26" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
       <c r="N26" s="25"/>
       <c r="O26" s="25"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="W26" s="9"/>
-      <c r="X26" s="9"/>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AH26" s="9"/>
-      <c r="AI26" s="9"/>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-      <c r="AR26" s="9"/>
-      <c r="AS26" s="9"/>
-      <c r="AT26" s="9"/>
-      <c r="AU26" s="9"/>
-      <c r="AV26" s="9"/>
-      <c r="AW26" s="9"/>
-      <c r="AX26" s="9"/>
-      <c r="AY26" s="9"/>
-      <c r="AZ26" s="9"/>
-      <c r="BA26" s="9"/>
-      <c r="BB26" s="9"/>
-      <c r="BC26" s="9"/>
-      <c r="BD26" s="9"/>
-      <c r="BE26" s="9"/>
-      <c r="BF26" s="9"/>
-      <c r="BG26" s="9"/>
-      <c r="BH26" s="9"/>
-      <c r="BI26" s="9"/>
-      <c r="BJ26" s="9"/>
-      <c r="BK26" s="9"/>
-      <c r="BL26" s="9"/>
-      <c r="BM26" s="9"/>
-      <c r="BN26" s="9"/>
-      <c r="BO26" s="9"/>
-      <c r="BP26" s="9"/>
-      <c r="BQ26" s="9"/>
-      <c r="BR26" s="9"/>
-      <c r="BS26" s="9"/>
-      <c r="BT26" s="9"/>
-      <c r="BU26" s="9"/>
-      <c r="BV26" s="6"/>
-      <c r="BW26" s="53"/>
-      <c r="BX26" s="9"/>
-      <c r="BY26" s="9"/>
-      <c r="BZ26" s="9"/>
-      <c r="CA26" s="9"/>
-      <c r="CB26" s="9"/>
-      <c r="CC26" s="9"/>
-      <c r="CD26" s="9"/>
-      <c r="CE26" s="9"/>
-      <c r="CF26" s="9"/>
-      <c r="CG26" s="19"/>
-      <c r="CH26" s="69"/>
-      <c r="CI26" s="70"/>
-      <c r="CJ26" s="71"/>
-    </row>
-    <row r="27" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B27" s="19">
-        <v>8</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="20"/>
+      <c r="AB26" s="20"/>
+      <c r="AC26" s="20"/>
+      <c r="AD26" s="20"/>
+      <c r="AE26" s="20"/>
+      <c r="AF26" s="20"/>
+      <c r="AG26" s="20"/>
+      <c r="AH26" s="20"/>
+      <c r="AI26" s="20"/>
+      <c r="AJ26" s="20"/>
+      <c r="AK26" s="20"/>
+      <c r="AL26" s="20"/>
+      <c r="AM26" s="20"/>
+      <c r="AN26" s="20"/>
+      <c r="AO26" s="20"/>
+      <c r="AP26" s="20"/>
+      <c r="AQ26" s="19"/>
+      <c r="AR26" s="20"/>
+      <c r="AS26" s="20"/>
+      <c r="AT26" s="20"/>
+      <c r="AU26" s="20"/>
+      <c r="AV26" s="20"/>
+      <c r="AW26" s="20"/>
+      <c r="AX26" s="20"/>
+      <c r="AY26" s="20"/>
+      <c r="AZ26" s="20"/>
+      <c r="BA26" s="20"/>
+      <c r="BB26" s="20"/>
+      <c r="BC26" s="20"/>
+      <c r="BD26" s="20"/>
+      <c r="BE26" s="20"/>
+      <c r="BF26" s="20"/>
+      <c r="BG26" s="20"/>
+      <c r="BH26" s="20"/>
+      <c r="BI26" s="20"/>
+      <c r="BJ26" s="20"/>
+      <c r="BK26" s="20"/>
+      <c r="BL26" s="20"/>
+      <c r="BM26" s="20"/>
+      <c r="BN26" s="20"/>
+      <c r="BO26" s="20"/>
+      <c r="BP26" s="20"/>
+      <c r="BQ26" s="20"/>
+      <c r="BR26" s="20"/>
+      <c r="BS26" s="20"/>
+      <c r="BT26" s="20"/>
+      <c r="BU26" s="20"/>
+      <c r="BV26" s="20"/>
+      <c r="BW26" s="20"/>
+      <c r="BX26" s="20"/>
+      <c r="BY26" s="20"/>
+      <c r="BZ26" s="20"/>
+      <c r="CA26" s="20"/>
+      <c r="CB26" s="20"/>
+      <c r="CC26" s="20"/>
+      <c r="CD26" s="20"/>
+      <c r="CE26" s="20"/>
+      <c r="CF26" s="20"/>
+      <c r="CG26" s="20"/>
+      <c r="CH26" s="17"/>
+      <c r="CI26" s="17"/>
+      <c r="CJ26" s="17"/>
+    </row>
+    <row r="27" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
       <c r="N27" s="25"/>
       <c r="O27" s="25"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
-      <c r="AG27" s="9"/>
-      <c r="AH27" s="9"/>
-      <c r="AI27" s="9"/>
-      <c r="AJ27" s="9"/>
-      <c r="AK27" s="9"/>
-      <c r="AL27" s="9"/>
-      <c r="AM27" s="9"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="9"/>
-      <c r="AP27" s="9"/>
-      <c r="AR27" s="9"/>
-      <c r="AS27" s="9"/>
-      <c r="AT27" s="9"/>
-      <c r="AU27" s="9"/>
-      <c r="AV27" s="9"/>
-      <c r="AW27" s="9"/>
-      <c r="AX27" s="9"/>
-      <c r="AY27" s="9"/>
-      <c r="AZ27" s="9"/>
-      <c r="BA27" s="9"/>
-      <c r="BB27" s="9"/>
-      <c r="BC27" s="9"/>
-      <c r="BD27" s="9"/>
-      <c r="BE27" s="9"/>
-      <c r="BF27" s="9"/>
-      <c r="BG27" s="9"/>
-      <c r="BH27" s="9"/>
-      <c r="BI27" s="9"/>
-      <c r="BJ27" s="9"/>
-      <c r="BK27" s="9"/>
-      <c r="BL27" s="9"/>
-      <c r="BM27" s="9"/>
-      <c r="BN27" s="9"/>
-      <c r="BO27" s="9"/>
-      <c r="BP27" s="9"/>
-      <c r="BQ27" s="9"/>
-      <c r="BR27" s="9"/>
-      <c r="BS27" s="9"/>
-      <c r="BT27" s="9"/>
-      <c r="BU27" s="9"/>
-      <c r="BV27" s="6"/>
-      <c r="BW27" s="53"/>
-      <c r="BX27" s="9"/>
-      <c r="BY27" s="9"/>
-      <c r="BZ27" s="9"/>
-      <c r="CA27" s="9"/>
-      <c r="CB27" s="9"/>
-      <c r="CC27" s="9"/>
-      <c r="CD27" s="9"/>
-      <c r="CE27" s="9"/>
-      <c r="CF27" s="9"/>
-      <c r="CG27" s="19"/>
-      <c r="CH27" s="69"/>
-      <c r="CI27" s="70"/>
-      <c r="CJ27" s="71"/>
-    </row>
-    <row r="28" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B28" s="19">
-        <v>9</v>
-      </c>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="20"/>
+      <c r="T27" s="20"/>
+      <c r="U27" s="20"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="20"/>
+      <c r="X27" s="20"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20"/>
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="20"/>
+      <c r="AG27" s="20"/>
+      <c r="AH27" s="20"/>
+      <c r="AI27" s="20"/>
+      <c r="AJ27" s="20"/>
+      <c r="AK27" s="20"/>
+      <c r="AL27" s="20"/>
+      <c r="AM27" s="20"/>
+      <c r="AN27" s="20"/>
+      <c r="AO27" s="20"/>
+      <c r="AP27" s="20"/>
+      <c r="AQ27" s="19"/>
+      <c r="AR27" s="20"/>
+      <c r="AS27" s="20"/>
+      <c r="AT27" s="20"/>
+      <c r="AU27" s="20"/>
+      <c r="AV27" s="20"/>
+      <c r="AW27" s="20"/>
+      <c r="AX27" s="20"/>
+      <c r="AY27" s="20"/>
+      <c r="AZ27" s="20"/>
+      <c r="BA27" s="20"/>
+      <c r="BB27" s="20"/>
+      <c r="BC27" s="20"/>
+      <c r="BD27" s="20"/>
+      <c r="BE27" s="20"/>
+      <c r="BF27" s="20"/>
+      <c r="BG27" s="20"/>
+      <c r="BH27" s="20"/>
+      <c r="BI27" s="20"/>
+      <c r="BJ27" s="20"/>
+      <c r="BK27" s="20"/>
+      <c r="BL27" s="20"/>
+      <c r="BM27" s="20"/>
+      <c r="BN27" s="20"/>
+      <c r="BO27" s="20"/>
+      <c r="BP27" s="20"/>
+      <c r="BQ27" s="20"/>
+      <c r="BR27" s="20"/>
+      <c r="BS27" s="20"/>
+      <c r="BT27" s="20"/>
+      <c r="BU27" s="20"/>
+      <c r="BV27" s="20"/>
+      <c r="BW27" s="20"/>
+      <c r="BX27" s="20"/>
+      <c r="BY27" s="20"/>
+      <c r="BZ27" s="20"/>
+      <c r="CA27" s="20"/>
+      <c r="CB27" s="20"/>
+      <c r="CC27" s="20"/>
+      <c r="CD27" s="20"/>
+      <c r="CE27" s="20"/>
+      <c r="CF27" s="20"/>
+      <c r="CG27" s="20"/>
+      <c r="CH27" s="17"/>
+      <c r="CI27" s="17"/>
+      <c r="CJ27" s="17"/>
+    </row>
+    <row r="28" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -3795,10 +3787,10 @@
       <c r="I28" s="20"/>
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="25"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
       <c r="R28" s="20"/>
@@ -3826,6 +3818,7 @@
       <c r="AN28" s="20"/>
       <c r="AO28" s="20"/>
       <c r="AP28" s="20"/>
+      <c r="AQ28" s="19"/>
       <c r="AR28" s="20"/>
       <c r="AS28" s="20"/>
       <c r="AT28" s="20"/>
@@ -3856,8 +3849,8 @@
       <c r="BS28" s="20"/>
       <c r="BT28" s="20"/>
       <c r="BU28" s="20"/>
-      <c r="BV28" s="66"/>
-      <c r="BW28" s="54"/>
+      <c r="BV28" s="20"/>
+      <c r="BW28" s="20"/>
       <c r="BX28" s="20"/>
       <c r="BY28" s="20"/>
       <c r="BZ28" s="20"/>
@@ -3867,101 +3860,100 @@
       <c r="CD28" s="20"/>
       <c r="CE28" s="20"/>
       <c r="CF28" s="20"/>
-      <c r="CG28" s="72"/>
-      <c r="CH28" s="69"/>
-      <c r="CI28" s="70"/>
-      <c r="CJ28" s="71"/>
-    </row>
-    <row r="29" s="1" customFormat="1" customHeight="1" spans="2:88">
-      <c r="B29" s="19">
-        <v>10</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="CG28" s="20"/>
+      <c r="CH28" s="17"/>
+      <c r="CI28" s="17"/>
+      <c r="CJ28" s="17"/>
+    </row>
+    <row r="29" s="1" customFormat="1" customHeight="1" spans="1:88">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
       <c r="L29" s="25"/>
       <c r="M29" s="25"/>
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
-      <c r="W29" s="9"/>
-      <c r="X29" s="9"/>
-      <c r="Y29" s="9"/>
-      <c r="Z29" s="9"/>
-      <c r="AA29" s="9"/>
-      <c r="AB29" s="9"/>
-      <c r="AC29" s="9"/>
-      <c r="AD29" s="9"/>
-      <c r="AE29" s="9"/>
-      <c r="AF29" s="9"/>
-      <c r="AG29" s="9"/>
-      <c r="AH29" s="9"/>
-      <c r="AI29" s="9"/>
-      <c r="AJ29" s="9"/>
-      <c r="AK29" s="9"/>
-      <c r="AL29" s="9"/>
-      <c r="AM29" s="6"/>
-      <c r="AN29" s="9"/>
-      <c r="AO29" s="9"/>
-      <c r="AP29" s="9"/>
-      <c r="AQ29" s="46"/>
-      <c r="AR29" s="9"/>
-      <c r="AS29" s="9"/>
-      <c r="AT29" s="9"/>
-      <c r="AU29" s="9"/>
-      <c r="AV29" s="9"/>
-      <c r="AW29" s="9"/>
-      <c r="AX29" s="9"/>
-      <c r="AY29" s="9"/>
-      <c r="AZ29" s="9"/>
-      <c r="BA29" s="9"/>
-      <c r="BB29" s="9"/>
-      <c r="BC29" s="9"/>
-      <c r="BD29" s="9"/>
-      <c r="BE29" s="9"/>
-      <c r="BF29" s="9"/>
-      <c r="BG29" s="9"/>
-      <c r="BH29" s="9"/>
-      <c r="BI29" s="9"/>
-      <c r="BJ29" s="9"/>
-      <c r="BK29" s="9"/>
-      <c r="BL29" s="9"/>
-      <c r="BM29" s="9"/>
-      <c r="BN29" s="9"/>
-      <c r="BO29" s="9"/>
-      <c r="BP29" s="9"/>
-      <c r="BQ29" s="9"/>
-      <c r="BR29" s="9"/>
-      <c r="BS29" s="9"/>
-      <c r="BT29" s="9"/>
-      <c r="BU29" s="9"/>
-      <c r="BV29" s="9"/>
-      <c r="BW29" s="9"/>
-      <c r="BX29" s="9"/>
-      <c r="BY29" s="9"/>
-      <c r="BZ29" s="9"/>
-      <c r="CA29" s="9"/>
-      <c r="CB29" s="9"/>
-      <c r="CC29" s="9"/>
-      <c r="CD29" s="9"/>
-      <c r="CE29" s="9"/>
-      <c r="CF29" s="9"/>
-      <c r="CG29" s="19"/>
-      <c r="CH29" s="69"/>
-      <c r="CI29" s="70"/>
-      <c r="CJ29" s="71"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="20"/>
+      <c r="T29" s="20"/>
+      <c r="U29" s="20"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="20"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20"/>
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="20"/>
+      <c r="AG29" s="20"/>
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
+      <c r="AJ29" s="20"/>
+      <c r="AK29" s="20"/>
+      <c r="AL29" s="20"/>
+      <c r="AM29" s="20"/>
+      <c r="AN29" s="20"/>
+      <c r="AO29" s="20"/>
+      <c r="AP29" s="20"/>
+      <c r="AQ29" s="20"/>
+      <c r="AR29" s="20"/>
+      <c r="AS29" s="20"/>
+      <c r="AT29" s="20"/>
+      <c r="AU29" s="20"/>
+      <c r="AV29" s="20"/>
+      <c r="AW29" s="20"/>
+      <c r="AX29" s="20"/>
+      <c r="AY29" s="20"/>
+      <c r="AZ29" s="20"/>
+      <c r="BA29" s="20"/>
+      <c r="BB29" s="20"/>
+      <c r="BC29" s="20"/>
+      <c r="BD29" s="20"/>
+      <c r="BE29" s="20"/>
+      <c r="BF29" s="20"/>
+      <c r="BG29" s="20"/>
+      <c r="BH29" s="20"/>
+      <c r="BI29" s="20"/>
+      <c r="BJ29" s="20"/>
+      <c r="BK29" s="20"/>
+      <c r="BL29" s="20"/>
+      <c r="BM29" s="20"/>
+      <c r="BN29" s="20"/>
+      <c r="BO29" s="20"/>
+      <c r="BP29" s="20"/>
+      <c r="BQ29" s="20"/>
+      <c r="BR29" s="20"/>
+      <c r="BS29" s="20"/>
+      <c r="BT29" s="20"/>
+      <c r="BU29" s="20"/>
+      <c r="BV29" s="20"/>
+      <c r="BW29" s="20"/>
+      <c r="BX29" s="20"/>
+      <c r="BY29" s="20"/>
+      <c r="BZ29" s="20"/>
+      <c r="CA29" s="20"/>
+      <c r="CB29" s="20"/>
+      <c r="CC29" s="20"/>
+      <c r="CD29" s="20"/>
+      <c r="CE29" s="20"/>
+      <c r="CF29" s="20"/>
+      <c r="CG29" s="20"/>
+      <c r="CH29" s="17"/>
+      <c r="CI29" s="17"/>
+      <c r="CJ29" s="17"/>
     </row>
     <row r="30" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B30" s="3"/>
@@ -3999,14 +3991,14 @@
       <c r="BY30" s="3"/>
       <c r="BZ30" s="3"/>
       <c r="CA30" s="3"/>
-      <c r="CB30" s="67"/>
-      <c r="CC30" s="67"/>
-      <c r="CD30" s="67"/>
-      <c r="CE30" s="67"/>
-      <c r="CF30" s="67"/>
-      <c r="CG30" s="67"/>
-      <c r="CH30" s="67"/>
-      <c r="CI30" s="67"/>
+      <c r="CB30" s="63"/>
+      <c r="CC30" s="63"/>
+      <c r="CD30" s="63"/>
+      <c r="CE30" s="63"/>
+      <c r="CF30" s="63"/>
+      <c r="CG30" s="63"/>
+      <c r="CH30" s="63"/>
+      <c r="CI30" s="63"/>
     </row>
     <row r="31" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B31" s="3"/>
@@ -4044,14 +4036,14 @@
       <c r="BY31" s="3"/>
       <c r="BZ31" s="3"/>
       <c r="CA31" s="3"/>
-      <c r="CB31" s="67"/>
-      <c r="CC31" s="67"/>
-      <c r="CD31" s="67"/>
-      <c r="CE31" s="67"/>
-      <c r="CF31" s="67"/>
-      <c r="CG31" s="67"/>
-      <c r="CH31" s="67"/>
-      <c r="CI31" s="67"/>
+      <c r="CB31" s="63"/>
+      <c r="CC31" s="63"/>
+      <c r="CD31" s="63"/>
+      <c r="CE31" s="63"/>
+      <c r="CF31" s="63"/>
+      <c r="CG31" s="63"/>
+      <c r="CH31" s="63"/>
+      <c r="CI31" s="63"/>
     </row>
     <row r="32" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B32" s="3"/>
@@ -4089,14 +4081,14 @@
       <c r="BY32" s="3"/>
       <c r="BZ32" s="3"/>
       <c r="CA32" s="3"/>
-      <c r="CB32" s="67"/>
-      <c r="CC32" s="67"/>
-      <c r="CD32" s="67"/>
-      <c r="CE32" s="67"/>
-      <c r="CF32" s="67"/>
-      <c r="CG32" s="67"/>
-      <c r="CH32" s="67"/>
-      <c r="CI32" s="67"/>
+      <c r="CB32" s="63"/>
+      <c r="CC32" s="63"/>
+      <c r="CD32" s="63"/>
+      <c r="CE32" s="63"/>
+      <c r="CF32" s="63"/>
+      <c r="CG32" s="63"/>
+      <c r="CH32" s="63"/>
+      <c r="CI32" s="63"/>
     </row>
     <row r="33" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B33" s="3"/>
@@ -4119,14 +4111,14 @@
       <c r="BY33" s="3"/>
       <c r="BZ33" s="3"/>
       <c r="CA33" s="3"/>
-      <c r="CB33" s="67"/>
-      <c r="CC33" s="67"/>
-      <c r="CD33" s="67"/>
-      <c r="CE33" s="67"/>
-      <c r="CF33" s="67"/>
-      <c r="CG33" s="67"/>
-      <c r="CH33" s="67"/>
-      <c r="CI33" s="67"/>
+      <c r="CB33" s="63"/>
+      <c r="CC33" s="63"/>
+      <c r="CD33" s="63"/>
+      <c r="CE33" s="63"/>
+      <c r="CF33" s="63"/>
+      <c r="CG33" s="63"/>
+      <c r="CH33" s="63"/>
+      <c r="CI33" s="63"/>
     </row>
     <row r="34" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B34" s="3"/>
@@ -4164,14 +4156,14 @@
       <c r="BY34" s="3"/>
       <c r="BZ34" s="3"/>
       <c r="CA34" s="3"/>
-      <c r="CB34" s="67"/>
-      <c r="CC34" s="67"/>
-      <c r="CD34" s="67"/>
-      <c r="CE34" s="67"/>
-      <c r="CF34" s="67"/>
-      <c r="CG34" s="67"/>
-      <c r="CH34" s="67"/>
-      <c r="CI34" s="67"/>
+      <c r="CB34" s="63"/>
+      <c r="CC34" s="63"/>
+      <c r="CD34" s="63"/>
+      <c r="CE34" s="63"/>
+      <c r="CF34" s="63"/>
+      <c r="CG34" s="63"/>
+      <c r="CH34" s="63"/>
+      <c r="CI34" s="63"/>
     </row>
     <row r="35" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B35" s="3"/>
@@ -4209,14 +4201,14 @@
       <c r="BY35" s="3"/>
       <c r="BZ35" s="3"/>
       <c r="CA35" s="3"/>
-      <c r="CB35" s="67"/>
-      <c r="CC35" s="67"/>
-      <c r="CD35" s="67"/>
-      <c r="CE35" s="67"/>
-      <c r="CF35" s="67"/>
-      <c r="CG35" s="67"/>
-      <c r="CH35" s="67"/>
-      <c r="CI35" s="67"/>
+      <c r="CB35" s="63"/>
+      <c r="CC35" s="63"/>
+      <c r="CD35" s="63"/>
+      <c r="CE35" s="63"/>
+      <c r="CF35" s="63"/>
+      <c r="CG35" s="63"/>
+      <c r="CH35" s="63"/>
+      <c r="CI35" s="63"/>
     </row>
     <row r="36" s="1" customFormat="1" customHeight="1" spans="2:87">
       <c r="B36" s="3"/>
@@ -4239,14 +4231,14 @@
       <c r="BY36" s="3"/>
       <c r="BZ36" s="3"/>
       <c r="CA36" s="3"/>
-      <c r="CB36" s="67"/>
-      <c r="CC36" s="67"/>
-      <c r="CD36" s="67"/>
-      <c r="CE36" s="67"/>
-      <c r="CF36" s="67"/>
-      <c r="CG36" s="67"/>
-      <c r="CH36" s="67"/>
-      <c r="CI36" s="67"/>
+      <c r="CB36" s="63"/>
+      <c r="CC36" s="63"/>
+      <c r="CD36" s="63"/>
+      <c r="CE36" s="63"/>
+      <c r="CF36" s="63"/>
+      <c r="CG36" s="63"/>
+      <c r="CH36" s="63"/>
+      <c r="CI36" s="63"/>
     </row>
     <row r="37" s="1" customFormat="1" customHeight="1" spans="75:87">
       <c r="BW37" s="3"/>
@@ -4254,14 +4246,14 @@
       <c r="BY37" s="3"/>
       <c r="BZ37" s="3"/>
       <c r="CA37" s="3"/>
-      <c r="CB37" s="67"/>
-      <c r="CC37" s="67"/>
-      <c r="CD37" s="67"/>
-      <c r="CE37" s="67"/>
-      <c r="CF37" s="67"/>
-      <c r="CG37" s="67"/>
-      <c r="CH37" s="67"/>
-      <c r="CI37" s="67"/>
+      <c r="CB37" s="63"/>
+      <c r="CC37" s="63"/>
+      <c r="CD37" s="63"/>
+      <c r="CE37" s="63"/>
+      <c r="CF37" s="63"/>
+      <c r="CG37" s="63"/>
+      <c r="CH37" s="63"/>
+      <c r="CI37" s="63"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="75:87">
       <c r="BW38" s="3"/>
@@ -6754,7 +6746,7 @@
       <c r="CI203" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="203">
+  <mergeCells count="73">
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="G3:L3"/>
     <mergeCell ref="M3:N3"/>
@@ -6811,136 +6803,6 @@
     <mergeCell ref="AN18:AP18"/>
     <mergeCell ref="B19:AP19"/>
     <mergeCell ref="AR19:CJ19"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="L20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="S20:W20"/>
-    <mergeCell ref="X20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="AG20:AI20"/>
-    <mergeCell ref="AJ20:AM20"/>
-    <mergeCell ref="AN20:AP20"/>
-    <mergeCell ref="BW20:BX20"/>
-    <mergeCell ref="BY20:BZ20"/>
-    <mergeCell ref="CH20:CJ20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="L21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="S21:W21"/>
-    <mergeCell ref="X21:AC21"/>
-    <mergeCell ref="AD21:AF21"/>
-    <mergeCell ref="AG21:AI21"/>
-    <mergeCell ref="AJ21:AM21"/>
-    <mergeCell ref="AN21:AP21"/>
-    <mergeCell ref="BW21:BX21"/>
-    <mergeCell ref="BY21:BZ21"/>
-    <mergeCell ref="CH21:CJ21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="L22:O22"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="S22:W22"/>
-    <mergeCell ref="X22:AC22"/>
-    <mergeCell ref="AD22:AF22"/>
-    <mergeCell ref="AG22:AI22"/>
-    <mergeCell ref="AJ22:AM22"/>
-    <mergeCell ref="AN22:AP22"/>
-    <mergeCell ref="BW22:BX22"/>
-    <mergeCell ref="BY22:BZ22"/>
-    <mergeCell ref="CH22:CJ22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="L23:O23"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="S23:W23"/>
-    <mergeCell ref="X23:AC23"/>
-    <mergeCell ref="AD23:AF23"/>
-    <mergeCell ref="AG23:AI23"/>
-    <mergeCell ref="AJ23:AM23"/>
-    <mergeCell ref="AN23:AP23"/>
-    <mergeCell ref="BW23:BX23"/>
-    <mergeCell ref="BY23:BZ23"/>
-    <mergeCell ref="CH23:CJ23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:W24"/>
-    <mergeCell ref="X24:AC24"/>
-    <mergeCell ref="AD24:AF24"/>
-    <mergeCell ref="AG24:AI24"/>
-    <mergeCell ref="AJ24:AM24"/>
-    <mergeCell ref="AN24:AP24"/>
-    <mergeCell ref="BW24:BX24"/>
-    <mergeCell ref="BY24:BZ24"/>
-    <mergeCell ref="CH24:CJ24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="S25:W25"/>
-    <mergeCell ref="X25:AC25"/>
-    <mergeCell ref="AD25:AF25"/>
-    <mergeCell ref="AG25:AI25"/>
-    <mergeCell ref="AJ25:AM25"/>
-    <mergeCell ref="AN25:AP25"/>
-    <mergeCell ref="BW25:BX25"/>
-    <mergeCell ref="BY25:BZ25"/>
-    <mergeCell ref="CH25:CJ25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="L26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="S26:W26"/>
-    <mergeCell ref="X26:AC26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="AG26:AI26"/>
-    <mergeCell ref="AJ26:AM26"/>
-    <mergeCell ref="AN26:AP26"/>
-    <mergeCell ref="BW26:BX26"/>
-    <mergeCell ref="BY26:BZ26"/>
-    <mergeCell ref="CH26:CJ26"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="S27:W27"/>
-    <mergeCell ref="X27:AC27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="AG27:AI27"/>
-    <mergeCell ref="AJ27:AM27"/>
-    <mergeCell ref="AN27:AP27"/>
-    <mergeCell ref="BW27:BX27"/>
-    <mergeCell ref="BY27:BZ27"/>
-    <mergeCell ref="CH27:CJ27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="S28:W28"/>
-    <mergeCell ref="X28:AC28"/>
-    <mergeCell ref="AD28:AF28"/>
-    <mergeCell ref="AG28:AI28"/>
-    <mergeCell ref="AJ28:AM28"/>
-    <mergeCell ref="AN28:AP28"/>
-    <mergeCell ref="BW28:BX28"/>
-    <mergeCell ref="BY28:BZ28"/>
-    <mergeCell ref="CH28:CJ28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="S29:W29"/>
-    <mergeCell ref="X29:AC29"/>
-    <mergeCell ref="AD29:AF29"/>
-    <mergeCell ref="AG29:AI29"/>
-    <mergeCell ref="AJ29:AM29"/>
-    <mergeCell ref="AN29:AP29"/>
-    <mergeCell ref="BW29:BX29"/>
-    <mergeCell ref="BY29:BZ29"/>
-    <mergeCell ref="CH29:CJ29"/>
     <mergeCell ref="CA17:CA18"/>
     <mergeCell ref="CB17:CB18"/>
     <mergeCell ref="CC17:CC18"/>

</xml_diff>